<commit_message>
Refreshed schematic and table
</commit_message>
<xml_diff>
--- a/StateTable/StateTable.xlsx
+++ b/StateTable/StateTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17295" windowHeight="6105"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1238" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1994" uniqueCount="150">
   <si>
     <t>PC_Enable</t>
   </si>
@@ -341,6 +341,9 @@
     <t>Restore</t>
   </si>
   <si>
+    <t>Trap</t>
+  </si>
+  <si>
     <t>Trap (True)</t>
   </si>
   <si>
@@ -378,6 +381,99 @@
   </si>
   <si>
     <t>tt enable</t>
+  </si>
+  <si>
+    <t>nop</t>
+  </si>
+  <si>
+    <t>rett</t>
+  </si>
+  <si>
+    <t>Dec CWP</t>
+  </si>
+  <si>
+    <t>rs1 +rs2</t>
+  </si>
+  <si>
+    <t>41</t>
+  </si>
+  <si>
+    <t>Store rd in reg and FC</t>
+  </si>
+  <si>
+    <t>110</t>
+  </si>
+  <si>
+    <t>Normal Fetch</t>
+  </si>
+  <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illegal </t>
+  </si>
+  <si>
+    <t>Flow Op</t>
+  </si>
+  <si>
+    <t>underflow</t>
+  </si>
+  <si>
+    <t>overflow</t>
+  </si>
+  <si>
+    <t>Send undeflow to FC</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>Store rd in reg</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>Send overflow to FC</t>
+  </si>
+  <si>
+    <t>52</t>
+  </si>
+  <si>
+    <t>Send underflow to FC</t>
+  </si>
+  <si>
+    <t>Memory</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>Store in MAR</t>
+  </si>
+  <si>
+    <t>Load</t>
+  </si>
+  <si>
+    <t>Enable Ram and Opcode</t>
+  </si>
+  <si>
+    <t>Enable MDR</t>
+  </si>
+  <si>
+    <t>Fetch MDR</t>
+  </si>
+  <si>
+    <t>Store MDR in rd</t>
+  </si>
+  <si>
+    <t>61</t>
   </si>
 </sst>
 </file>
@@ -707,13 +803,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AH79"/>
+  <dimension ref="A2:AL79"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="AI13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="AB41" sqref="AB41"/>
+      <selection pane="bottomRight" activeCell="AL16" sqref="AL16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -750,10 +846,12 @@
     <col min="32" max="32" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="6" style="1" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="1"/>
+    <col min="35" max="35" width="9.140625" style="1"/>
+    <col min="36" max="36" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
@@ -793,7 +891,7 @@
       <c r="AG2" s="4"/>
       <c r="AH2" s="4"/>
     </row>
-    <row r="3" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
@@ -824,10 +922,10 @@
         <v>62</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>6</v>
@@ -892,8 +990,11 @@
       <c r="AH3" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="AK3" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
-    <row r="4" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
         <v>28</v>
       </c>
@@ -940,7 +1041,7 @@
         <v>33</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>33</v>
@@ -994,7 +1095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>30</v>
       </c>
@@ -1044,7 +1145,7 @@
         <v>34</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R5" s="3" t="s">
         <v>33</v>
@@ -1098,7 +1199,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:34" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>74</v>
       </c>
@@ -1145,7 +1246,7 @@
         <v>34</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>33</v>
@@ -1199,7 +1300,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>36</v>
       </c>
@@ -1249,7 +1350,7 @@
         <v>33</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R7" s="3" t="s">
         <v>33</v>
@@ -1303,7 +1404,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -1353,7 +1454,7 @@
         <v>33</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R8" s="3" t="s">
         <v>33</v>
@@ -1407,7 +1508,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>40</v>
       </c>
@@ -1457,7 +1558,7 @@
         <v>33</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>33</v>
@@ -1511,12 +1612,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>51</v>
+        <v>119</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>84</v>
@@ -1525,10 +1626,10 @@
         <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>27</v>
@@ -1561,7 +1662,7 @@
         <v>33</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>33</v>
@@ -1594,10 +1695,10 @@
         <v>27</v>
       </c>
       <c r="AB10" s="3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="AC10" s="3" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="AD10" s="3" t="s">
         <v>23</v>
@@ -1615,7 +1716,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>41</v>
       </c>
@@ -1665,7 +1766,7 @@
         <v>33</v>
       </c>
       <c r="Q11" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R11" s="3" t="s">
         <v>33</v>
@@ -1719,7 +1820,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>43</v>
       </c>
@@ -1769,7 +1870,7 @@
         <v>33</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R12" s="3" t="s">
         <v>33</v>
@@ -1823,7 +1924,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>44</v>
       </c>
@@ -1873,7 +1974,7 @@
         <v>33</v>
       </c>
       <c r="Q13" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R13" s="3" t="s">
         <v>33</v>
@@ -1927,7 +2028,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>45</v>
       </c>
@@ -1977,7 +2078,7 @@
         <v>34</v>
       </c>
       <c r="Q14" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R14" s="3" t="s">
         <v>33</v>
@@ -2031,7 +2132,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3" t="s">
         <v>59</v>
@@ -2079,7 +2180,7 @@
         <v>34</v>
       </c>
       <c r="Q15" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R15" s="3" t="s">
         <v>33</v>
@@ -2133,7 +2234,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>49</v>
       </c>
@@ -2183,7 +2284,7 @@
         <v>47</v>
       </c>
       <c r="Q16" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R16" s="3" t="s">
         <v>33</v>
@@ -2236,8 +2337,15 @@
       <c r="AH16" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AJ16" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AK16" s="2">
+        <v>0</v>
+      </c>
+      <c r="AL16" s="2"/>
     </row>
-    <row r="17" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>71</v>
@@ -2285,7 +2393,7 @@
         <v>47</v>
       </c>
       <c r="Q17" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R17" s="3" t="s">
         <v>33</v>
@@ -2338,8 +2446,14 @@
       <c r="AH17" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AJ17" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="AK17" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="3" t="s">
         <v>68</v>
@@ -2387,7 +2501,7 @@
         <v>34</v>
       </c>
       <c r="Q18" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R18" s="3" t="s">
         <v>33</v>
@@ -2440,8 +2554,14 @@
       <c r="AH18" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AJ18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AK18" s="2">
+        <v>10</v>
+      </c>
     </row>
-    <row r="19" spans="1:34" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
       <c r="B19" s="3" t="s">
         <v>75</v>
@@ -2489,7 +2609,7 @@
         <v>34</v>
       </c>
       <c r="Q19" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R19" s="3" t="s">
         <v>33</v>
@@ -2542,8 +2662,14 @@
       <c r="AH19" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AJ19" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AK19" s="2">
+        <v>11</v>
+      </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="3" t="s">
         <v>51</v>
@@ -2591,7 +2717,7 @@
         <v>34</v>
       </c>
       <c r="Q20" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>33</v>
@@ -2644,8 +2770,14 @@
       <c r="AH20" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AJ20" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK20" s="2">
+        <v>100</v>
+      </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>53</v>
       </c>
@@ -2695,7 +2827,7 @@
         <v>33</v>
       </c>
       <c r="Q21" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R21" s="3" t="s">
         <v>33</v>
@@ -2748,8 +2880,15 @@
       <c r="AH21" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AJ21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="AK21" s="2">
+        <v>101</v>
+      </c>
+      <c r="AL21" s="2"/>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A22" s="3"/>
       <c r="B22" s="3" t="s">
         <v>58</v>
@@ -2797,7 +2936,7 @@
         <v>34</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R22" s="3" t="s">
         <v>33</v>
@@ -2850,8 +2989,14 @@
       <c r="AH22" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AJ22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK22" s="2">
+        <v>110</v>
+      </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="3" t="s">
         <v>64</v>
@@ -2899,7 +3044,7 @@
         <v>33</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R23" s="3" t="s">
         <v>33</v>
@@ -2914,7 +3059,7 @@
         <v>48</v>
       </c>
       <c r="V23" s="3" t="s">
-        <v>55</v>
+        <v>27</v>
       </c>
       <c r="W23" s="3" t="s">
         <v>27</v>
@@ -2952,8 +3097,14 @@
       <c r="AH23" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AJ23" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK23" s="1">
+        <v>111</v>
+      </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>69</v>
       </c>
@@ -3003,7 +3154,7 @@
         <v>47</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R24" s="3" t="s">
         <v>33</v>
@@ -3056,8 +3207,14 @@
       <c r="AH24" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AJ24" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AK24" s="1">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A25" s="3"/>
       <c r="B25" s="3" t="s">
         <v>72</v>
@@ -3105,7 +3262,7 @@
         <v>11</v>
       </c>
       <c r="Q25" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R25" s="3" t="s">
         <v>33</v>
@@ -3158,8 +3315,14 @@
       <c r="AH25" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="AJ25" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AK25" s="1">
+        <v>1001</v>
+      </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>54</v>
       </c>
@@ -3209,7 +3372,7 @@
         <v>33</v>
       </c>
       <c r="Q26" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R26" s="3" t="s">
         <v>33</v>
@@ -3263,7 +3426,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
         <v>73</v>
       </c>
@@ -3310,7 +3473,7 @@
         <v>33</v>
       </c>
       <c r="Q27" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R27" s="3" t="s">
         <v>33</v>
@@ -3364,7 +3527,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>51</v>
       </c>
@@ -3411,7 +3574,7 @@
         <v>33</v>
       </c>
       <c r="Q28" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R28" s="3" t="s">
         <v>33</v>
@@ -3465,7 +3628,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>58</v>
       </c>
@@ -3515,7 +3678,7 @@
         <v>34</v>
       </c>
       <c r="Q29" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R29" s="3" t="s">
         <v>33</v>
@@ -3569,7 +3732,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
         <v>73</v>
       </c>
@@ -3616,7 +3779,7 @@
         <v>33</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R30" s="3" t="s">
         <v>33</v>
@@ -3670,7 +3833,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>51</v>
       </c>
@@ -3717,7 +3880,7 @@
         <v>33</v>
       </c>
       <c r="Q31" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R31" s="3" t="s">
         <v>33</v>
@@ -3771,12 +3934,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C32" s="1">
         <v>28</v>
@@ -3821,7 +3984,7 @@
         <v>33</v>
       </c>
       <c r="Q32" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R32" s="3" t="s">
         <v>34</v>
@@ -3875,9 +4038,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C33" s="1">
         <v>29</v>
@@ -3922,7 +4085,7 @@
         <v>33</v>
       </c>
       <c r="Q33" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R33" s="3" t="s">
         <v>33</v>
@@ -3976,9 +4139,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C34" s="1">
         <v>30</v>
@@ -4023,7 +4186,7 @@
         <v>47</v>
       </c>
       <c r="Q34" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R34" s="3" t="s">
         <v>33</v>
@@ -4077,9 +4240,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C35" s="1">
         <v>31</v>
@@ -4124,7 +4287,7 @@
         <v>33</v>
       </c>
       <c r="Q35" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R35" s="3" t="s">
         <v>33</v>
@@ -4136,7 +4299,7 @@
         <v>27</v>
       </c>
       <c r="U35" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="V35" s="3" t="s">
         <v>25</v>
@@ -4178,9 +4341,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C36" s="2">
         <v>32</v>
@@ -4222,10 +4385,10 @@
         <v>33</v>
       </c>
       <c r="P36" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q36" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R36" s="3" t="s">
         <v>33</v>
@@ -4279,9 +4442,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="37" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C37" s="2">
         <v>33</v>
@@ -4326,7 +4489,7 @@
         <v>33</v>
       </c>
       <c r="Q37" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R37" s="3" t="s">
         <v>33</v>
@@ -4338,7 +4501,7 @@
         <v>27</v>
       </c>
       <c r="U37" s="3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="V37" s="3" t="s">
         <v>25</v>
@@ -4380,7 +4543,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
         <v>54</v>
       </c>
@@ -4427,7 +4590,7 @@
         <v>33</v>
       </c>
       <c r="Q38" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R38" s="3" t="s">
         <v>33</v>
@@ -4481,7 +4644,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
         <v>58</v>
       </c>
@@ -4528,7 +4691,7 @@
         <v>34</v>
       </c>
       <c r="Q39" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R39" s="3" t="s">
         <v>33</v>
@@ -4582,9 +4745,9 @@
         <v>27</v>
       </c>
     </row>
-    <row r="40" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C40" s="1">
         <v>36</v>
@@ -4629,7 +4792,7 @@
         <v>33</v>
       </c>
       <c r="Q40" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R40" s="3" t="s">
         <v>33</v>
@@ -4683,7 +4846,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="41" spans="2:34" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:34" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
         <v>51</v>
       </c>
@@ -4730,7 +4893,7 @@
         <v>33</v>
       </c>
       <c r="Q41" s="3" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="R41" s="3" t="s">
         <v>33</v>
@@ -4757,7 +4920,7 @@
         <v>26</v>
       </c>
       <c r="Z41" s="3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AA41" s="3" t="s">
         <v>27</v>
@@ -4784,799 +4947,2458 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-      <c r="K42" s="3"/>
-      <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
-      <c r="N42" s="3"/>
-      <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
-      <c r="R42" s="3"/>
-      <c r="S42" s="3"/>
-      <c r="T42" s="3"/>
-      <c r="U42" s="3"/>
-      <c r="V42" s="3"/>
-      <c r="W42" s="3"/>
-      <c r="X42" s="3"/>
-      <c r="Y42" s="3"/>
-      <c r="Z42" s="3"/>
-      <c r="AA42" s="3"/>
-      <c r="AB42" s="3"/>
-      <c r="AC42" s="3"/>
-      <c r="AD42" s="3"/>
-      <c r="AE42" s="3"/>
-      <c r="AF42" s="3"/>
-      <c r="AG42" s="3"/>
-      <c r="AH42" s="3"/>
+    <row r="42" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C42" s="1">
+        <v>38</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R42" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X42" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y42" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z42" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC42" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD42" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG42" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH42" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="43" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
-      <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
-      <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
-      <c r="V43" s="3"/>
-      <c r="W43" s="3"/>
-      <c r="X43" s="3"/>
-      <c r="Y43" s="3"/>
-      <c r="Z43" s="3"/>
-      <c r="AA43" s="3"/>
-      <c r="AB43" s="3"/>
-      <c r="AC43" s="3"/>
-      <c r="AD43" s="3"/>
-      <c r="AE43" s="3"/>
-      <c r="AF43" s="3"/>
-      <c r="AG43" s="3"/>
-      <c r="AH43" s="3"/>
+    <row r="43" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C43" s="1">
+        <v>39</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R43" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T43" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="U43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X43" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y43" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z43" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC43" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG43" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH43" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="44" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
-      <c r="V44" s="3"/>
-      <c r="W44" s="3"/>
-      <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
-      <c r="Z44" s="3"/>
-      <c r="AA44" s="3"/>
-      <c r="AB44" s="3"/>
-      <c r="AC44" s="3"/>
-      <c r="AD44" s="3"/>
-      <c r="AE44" s="3"/>
-      <c r="AF44" s="3"/>
-      <c r="AG44" s="3"/>
-      <c r="AH44" s="3"/>
+    <row r="44" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="1">
+        <v>40</v>
+      </c>
+      <c r="D44" s="3">
+        <v>0</v>
+      </c>
+      <c r="E44" s="3">
+        <v>0</v>
+      </c>
+      <c r="F44" s="3">
+        <v>0</v>
+      </c>
+      <c r="G44" s="3">
+        <v>0</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3">
+        <v>0</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N44" s="3">
+        <v>0</v>
+      </c>
+      <c r="O44" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P44" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R44" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V44" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W44" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X44" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y44" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC44" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD44" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG44" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH44" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="45" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
-      <c r="R45" s="3"/>
-      <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
-      <c r="U45" s="3"/>
-      <c r="V45" s="3"/>
-      <c r="W45" s="3"/>
-      <c r="X45" s="3"/>
-      <c r="Y45" s="3"/>
-      <c r="Z45" s="3"/>
-      <c r="AA45" s="3"/>
-      <c r="AB45" s="3"/>
-      <c r="AC45" s="3"/>
-      <c r="AD45" s="3"/>
-      <c r="AE45" s="3"/>
-      <c r="AF45" s="3"/>
-      <c r="AG45" s="3"/>
-      <c r="AH45" s="3"/>
+    <row r="45" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O45" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P45" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R45" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V45" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X45" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y45" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC45" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD45" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG45" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH45" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="46" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="D46" s="3"/>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-      <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3"/>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
-      <c r="R46" s="3"/>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
-      <c r="U46" s="3"/>
-      <c r="V46" s="3"/>
-      <c r="W46" s="3"/>
-      <c r="X46" s="3"/>
-      <c r="Y46" s="3"/>
-      <c r="Z46" s="3"/>
-      <c r="AA46" s="3"/>
-      <c r="AB46" s="3"/>
-      <c r="AC46" s="3"/>
-      <c r="AD46" s="3"/>
-      <c r="AE46" s="3"/>
-      <c r="AF46" s="3"/>
-      <c r="AG46" s="3"/>
-      <c r="AH46" s="3"/>
+    <row r="46" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C46" s="1">
+        <v>42</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I46" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K46" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="L46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R46" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X46" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y46" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC46" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD46" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG46" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH46" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="47" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-      <c r="K47" s="3"/>
-      <c r="L47" s="3"/>
-      <c r="M47" s="3"/>
-      <c r="N47" s="3"/>
-      <c r="O47" s="3"/>
-      <c r="P47" s="3"/>
-      <c r="Q47" s="3"/>
-      <c r="R47" s="3"/>
-      <c r="S47" s="3"/>
-      <c r="T47" s="3"/>
-      <c r="U47" s="3"/>
-      <c r="V47" s="3"/>
-      <c r="W47" s="3"/>
-      <c r="X47" s="3"/>
-      <c r="Y47" s="3"/>
-      <c r="Z47" s="3"/>
-      <c r="AA47" s="3"/>
-      <c r="AB47" s="3"/>
-      <c r="AC47" s="3"/>
-      <c r="AD47" s="3"/>
-      <c r="AE47" s="3"/>
-      <c r="AF47" s="3"/>
-      <c r="AG47" s="3"/>
-      <c r="AH47" s="3"/>
+    <row r="47" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="1">
+        <v>43</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O47" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P47" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R47" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X47" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y47" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z47" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="AA47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB47" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC47" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD47" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH47" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="48" spans="2:34" x14ac:dyDescent="0.25">
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3"/>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3"/>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="3"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="3"/>
-      <c r="P48" s="3"/>
-      <c r="Q48" s="3"/>
-      <c r="R48" s="3"/>
-      <c r="S48" s="3"/>
-      <c r="T48" s="3"/>
-      <c r="U48" s="3"/>
-      <c r="V48" s="3"/>
-      <c r="W48" s="3"/>
-      <c r="X48" s="3"/>
-      <c r="Y48" s="3"/>
-      <c r="Z48" s="3"/>
-      <c r="AA48" s="3"/>
-      <c r="AB48" s="3"/>
-      <c r="AC48" s="3"/>
-      <c r="AD48" s="3"/>
-      <c r="AE48" s="3"/>
-      <c r="AF48" s="3"/>
-      <c r="AG48" s="3"/>
-      <c r="AH48" s="3"/>
+    <row r="48" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C48" s="1">
+        <v>44</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F48" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O48" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P48" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X48" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y48" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z48" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB48" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC48" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD48" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF48" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG48" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH48" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="49" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="P49" s="3"/>
-      <c r="Q49" s="3"/>
-      <c r="R49" s="3"/>
-      <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
-      <c r="V49" s="3"/>
-      <c r="W49" s="3"/>
-      <c r="X49" s="3"/>
-      <c r="Y49" s="3"/>
-      <c r="Z49" s="3"/>
-      <c r="AA49" s="3"/>
-      <c r="AB49" s="3"/>
-      <c r="AC49" s="3"/>
-      <c r="AD49" s="3"/>
-      <c r="AE49" s="3"/>
-      <c r="AF49" s="3"/>
-      <c r="AG49" s="3"/>
-      <c r="AH49" s="3"/>
+    <row r="49" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C49" s="1">
+        <v>45</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O49" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P49" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R49" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S49" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="T49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X49" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y49" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z49" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC49" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD49" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG49" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH49" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="50" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D50" s="3"/>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="3"/>
-      <c r="L50" s="3"/>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3"/>
-      <c r="O50" s="3"/>
-      <c r="P50" s="3"/>
-      <c r="Q50" s="3"/>
-      <c r="R50" s="3"/>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
-      <c r="U50" s="3"/>
-      <c r="V50" s="3"/>
-      <c r="W50" s="3"/>
-      <c r="X50" s="3"/>
-      <c r="Y50" s="3"/>
-      <c r="Z50" s="3"/>
-      <c r="AA50" s="3"/>
-      <c r="AB50" s="3"/>
-      <c r="AC50" s="3"/>
-      <c r="AD50" s="3"/>
-      <c r="AE50" s="3"/>
-      <c r="AF50" s="3"/>
-      <c r="AG50" s="3"/>
-      <c r="AH50" s="3"/>
+    <row r="50" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B50" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="2">
+        <v>46</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0</v>
+      </c>
+      <c r="G50" s="3">
+        <v>0</v>
+      </c>
+      <c r="H50" s="3">
+        <v>0</v>
+      </c>
+      <c r="I50" s="3">
+        <v>0</v>
+      </c>
+      <c r="J50" s="3">
+        <v>0</v>
+      </c>
+      <c r="K50" s="3">
+        <v>0</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N50" s="3">
+        <v>0</v>
+      </c>
+      <c r="O50" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P50" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R50" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V50" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W50" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X50" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y50" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z50" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC50" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD50" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG50" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH50" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="51" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D51" s="3"/>
-      <c r="E51" s="3"/>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="3"/>
-      <c r="I51" s="3"/>
-      <c r="J51" s="3"/>
-      <c r="K51" s="3"/>
-      <c r="L51" s="3"/>
-      <c r="M51" s="3"/>
-      <c r="N51" s="3"/>
-      <c r="O51" s="3"/>
-      <c r="P51" s="3"/>
-      <c r="Q51" s="3"/>
-      <c r="R51" s="3"/>
-      <c r="S51" s="3"/>
-      <c r="T51" s="3"/>
-      <c r="U51" s="3"/>
-      <c r="V51" s="3"/>
-      <c r="W51" s="3"/>
-      <c r="X51" s="3"/>
-      <c r="Y51" s="3"/>
-      <c r="Z51" s="3"/>
-      <c r="AA51" s="3"/>
-      <c r="AB51" s="3"/>
-      <c r="AC51" s="3"/>
-      <c r="AD51" s="3"/>
-      <c r="AE51" s="3"/>
-      <c r="AF51" s="3"/>
-      <c r="AG51" s="3"/>
-      <c r="AH51" s="3"/>
+    <row r="51" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B51" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O51" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P51" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R51" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V51" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X51" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y51" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z51" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC51" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD51" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG51" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH51" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="52" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3"/>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3"/>
-      <c r="Q52" s="3"/>
-      <c r="R52" s="3"/>
-      <c r="S52" s="3"/>
-      <c r="T52" s="3"/>
-      <c r="U52" s="3"/>
-      <c r="V52" s="3"/>
-      <c r="W52" s="3"/>
-      <c r="X52" s="3"/>
-      <c r="Y52" s="3"/>
-      <c r="Z52" s="3"/>
-      <c r="AA52" s="3"/>
-      <c r="AB52" s="3"/>
-      <c r="AC52" s="3"/>
-      <c r="AD52" s="3"/>
-      <c r="AE52" s="3"/>
-      <c r="AF52" s="3"/>
-      <c r="AG52" s="3"/>
-      <c r="AH52" s="3"/>
+    <row r="52" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B52" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C52" s="2">
+        <v>48</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I52" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O52" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P52" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R52" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X52" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y52" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC52" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD52" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH52" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="53" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D53" s="3"/>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3"/>
-      <c r="O53" s="3"/>
-      <c r="P53" s="3"/>
-      <c r="Q53" s="3"/>
-      <c r="R53" s="3"/>
-      <c r="S53" s="3"/>
-      <c r="T53" s="3"/>
-      <c r="U53" s="3"/>
-      <c r="V53" s="3"/>
-      <c r="W53" s="3"/>
-      <c r="X53" s="3"/>
-      <c r="Y53" s="3"/>
-      <c r="Z53" s="3"/>
-      <c r="AA53" s="3"/>
-      <c r="AB53" s="3"/>
-      <c r="AC53" s="3"/>
-      <c r="AD53" s="3"/>
-      <c r="AE53" s="3"/>
-      <c r="AF53" s="3"/>
-      <c r="AG53" s="3"/>
-      <c r="AH53" s="3"/>
+    <row r="53" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C53" s="1">
+        <v>49</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F53" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O53" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P53" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R53" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X53" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y53" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z53" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB53" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC53" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD53" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF53" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG53" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AH53" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="54" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D54" s="3"/>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-      <c r="K54" s="3"/>
-      <c r="L54" s="3"/>
-      <c r="M54" s="3"/>
-      <c r="N54" s="3"/>
-      <c r="O54" s="3"/>
-      <c r="P54" s="3"/>
-      <c r="Q54" s="3"/>
-      <c r="R54" s="3"/>
-      <c r="S54" s="3"/>
-      <c r="T54" s="3"/>
-      <c r="U54" s="3"/>
-      <c r="V54" s="3"/>
-      <c r="W54" s="3"/>
-      <c r="X54" s="3"/>
-      <c r="Y54" s="3"/>
-      <c r="Z54" s="3"/>
-      <c r="AA54" s="3"/>
-      <c r="AB54" s="3"/>
-      <c r="AC54" s="3"/>
-      <c r="AD54" s="3"/>
-      <c r="AE54" s="3"/>
-      <c r="AF54" s="3"/>
-      <c r="AG54" s="3"/>
-      <c r="AH54" s="3"/>
+    <row r="54" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="C54" s="2">
+        <v>50</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R54" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T54" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="U54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X54" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y54" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC54" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD54" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG54" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH54" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="55" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3"/>
-      <c r="O55" s="3"/>
-      <c r="P55" s="3"/>
-      <c r="Q55" s="3"/>
-      <c r="R55" s="3"/>
-      <c r="S55" s="3"/>
-      <c r="T55" s="3"/>
-      <c r="U55" s="3"/>
-      <c r="V55" s="3"/>
-      <c r="W55" s="3"/>
-      <c r="X55" s="3"/>
-      <c r="Y55" s="3"/>
-      <c r="Z55" s="3"/>
-      <c r="AA55" s="3"/>
-      <c r="AB55" s="3"/>
-      <c r="AC55" s="3"/>
-      <c r="AD55" s="3"/>
-      <c r="AE55" s="3"/>
-      <c r="AF55" s="3"/>
-      <c r="AG55" s="3"/>
-      <c r="AH55" s="3"/>
+    <row r="55" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C55" s="2">
+        <v>51</v>
+      </c>
+      <c r="D55" s="3">
+        <v>0</v>
+      </c>
+      <c r="E55" s="3">
+        <v>0</v>
+      </c>
+      <c r="F55" s="3">
+        <v>0</v>
+      </c>
+      <c r="G55" s="3">
+        <v>0</v>
+      </c>
+      <c r="H55" s="3">
+        <v>0</v>
+      </c>
+      <c r="I55" s="3">
+        <v>0</v>
+      </c>
+      <c r="J55" s="3">
+        <v>0</v>
+      </c>
+      <c r="K55" s="3">
+        <v>0</v>
+      </c>
+      <c r="L55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N55" s="3">
+        <v>0</v>
+      </c>
+      <c r="O55" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P55" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R55" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V55" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W55" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X55" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y55" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z55" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC55" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD55" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG55" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH55" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="56" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="3"/>
-      <c r="G56" s="3"/>
-      <c r="H56" s="3"/>
-      <c r="I56" s="3"/>
-      <c r="J56" s="3"/>
-      <c r="K56" s="3"/>
-      <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
-      <c r="N56" s="3"/>
-      <c r="O56" s="3"/>
-      <c r="P56" s="3"/>
-      <c r="Q56" s="3"/>
-      <c r="R56" s="3"/>
-      <c r="S56" s="3"/>
-      <c r="T56" s="3"/>
-      <c r="U56" s="3"/>
-      <c r="V56" s="3"/>
-      <c r="W56" s="3"/>
-      <c r="X56" s="3"/>
-      <c r="Y56" s="3"/>
-      <c r="Z56" s="3"/>
-      <c r="AA56" s="3"/>
-      <c r="AB56" s="3"/>
-      <c r="AC56" s="3"/>
-      <c r="AD56" s="3"/>
-      <c r="AE56" s="3"/>
-      <c r="AF56" s="3"/>
-      <c r="AG56" s="3"/>
-      <c r="AH56" s="3"/>
+    <row r="56" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O56" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P56" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R56" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V56" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X56" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y56" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z56" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC56" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD56" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG56" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH56" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="57" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-      <c r="K57" s="3"/>
-      <c r="L57" s="3"/>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3"/>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3"/>
-      <c r="Q57" s="3"/>
-      <c r="R57" s="3"/>
-      <c r="S57" s="3"/>
-      <c r="T57" s="3"/>
-      <c r="U57" s="3"/>
-      <c r="V57" s="3"/>
-      <c r="W57" s="3"/>
-      <c r="X57" s="3"/>
-      <c r="Y57" s="3"/>
-      <c r="Z57" s="3"/>
-      <c r="AA57" s="3"/>
-      <c r="AB57" s="3"/>
-      <c r="AC57" s="3"/>
-      <c r="AD57" s="3"/>
-      <c r="AE57" s="3"/>
-      <c r="AF57" s="3"/>
-      <c r="AG57" s="3"/>
-      <c r="AH57" s="3"/>
+    <row r="57" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C57" s="2">
+        <v>53</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I57" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O57" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P57" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R57" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X57" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y57" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z57" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC57" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD57" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG57" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH57" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="58" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-      <c r="K58" s="3"/>
-      <c r="L58" s="3"/>
-      <c r="M58" s="3"/>
-      <c r="N58" s="3"/>
-      <c r="O58" s="3"/>
-      <c r="P58" s="3"/>
-      <c r="Q58" s="3"/>
-      <c r="R58" s="3"/>
-      <c r="S58" s="3"/>
-      <c r="T58" s="3"/>
-      <c r="U58" s="3"/>
-      <c r="V58" s="3"/>
-      <c r="W58" s="3"/>
-      <c r="X58" s="3"/>
-      <c r="Y58" s="3"/>
-      <c r="Z58" s="3"/>
-      <c r="AA58" s="3"/>
-      <c r="AB58" s="3"/>
-      <c r="AC58" s="3"/>
-      <c r="AD58" s="3"/>
-      <c r="AE58" s="3"/>
-      <c r="AF58" s="3"/>
-      <c r="AG58" s="3"/>
-      <c r="AH58" s="3"/>
+    <row r="58" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C58" s="2">
+        <v>54</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F58" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O58" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P58" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X58" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y58" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z58" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="AA58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB58" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC58" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD58" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF58" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG58" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH58" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="59" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D59" s="3"/>
-      <c r="E59" s="3"/>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="3"/>
-      <c r="I59" s="3"/>
-      <c r="J59" s="3"/>
-      <c r="K59" s="3"/>
-      <c r="L59" s="3"/>
-      <c r="M59" s="3"/>
-      <c r="N59" s="3"/>
-      <c r="O59" s="3"/>
-      <c r="P59" s="3"/>
-      <c r="Q59" s="3"/>
-      <c r="R59" s="3"/>
-      <c r="S59" s="3"/>
-      <c r="T59" s="3"/>
-      <c r="U59" s="3"/>
-      <c r="V59" s="3"/>
-      <c r="W59" s="3"/>
-      <c r="X59" s="3"/>
-      <c r="Y59" s="3"/>
-      <c r="Z59" s="3"/>
-      <c r="AA59" s="3"/>
-      <c r="AB59" s="3"/>
-      <c r="AC59" s="3"/>
-      <c r="AD59" s="3"/>
-      <c r="AE59" s="3"/>
-      <c r="AF59" s="3"/>
-      <c r="AG59" s="3"/>
-      <c r="AH59" s="3"/>
+    <row r="59" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="C59" s="2">
+        <v>55</v>
+      </c>
+      <c r="D59" s="3">
+        <v>0</v>
+      </c>
+      <c r="E59" s="3">
+        <v>0</v>
+      </c>
+      <c r="F59" s="3">
+        <v>0</v>
+      </c>
+      <c r="G59" s="3">
+        <v>0</v>
+      </c>
+      <c r="H59" s="3">
+        <v>0</v>
+      </c>
+      <c r="I59" s="3">
+        <v>0</v>
+      </c>
+      <c r="J59" s="3">
+        <v>0</v>
+      </c>
+      <c r="K59" s="3">
+        <v>0</v>
+      </c>
+      <c r="L59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N59" s="3">
+        <v>0</v>
+      </c>
+      <c r="O59" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P59" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R59" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V59" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W59" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X59" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y59" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z59" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC59" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD59" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AE59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG59" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH59" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="60" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D60" s="3"/>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-      <c r="K60" s="3"/>
-      <c r="L60" s="3"/>
-      <c r="M60" s="3"/>
-      <c r="N60" s="3"/>
-      <c r="O60" s="3"/>
-      <c r="P60" s="3"/>
-      <c r="Q60" s="3"/>
-      <c r="R60" s="3"/>
-      <c r="S60" s="3"/>
-      <c r="T60" s="3"/>
-      <c r="U60" s="3"/>
-      <c r="V60" s="3"/>
-      <c r="W60" s="3"/>
-      <c r="X60" s="3"/>
-      <c r="Y60" s="3"/>
-      <c r="Z60" s="3"/>
-      <c r="AA60" s="3"/>
-      <c r="AB60" s="3"/>
-      <c r="AC60" s="3"/>
-      <c r="AD60" s="3"/>
-      <c r="AE60" s="3"/>
-      <c r="AF60" s="3"/>
-      <c r="AG60" s="3"/>
-      <c r="AH60" s="3"/>
+    <row r="60" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O60" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P60" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R60" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V60" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="W60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X60" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y60" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z60" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC60" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD60" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG60" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH60" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="61" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="N61" s="3"/>
-      <c r="O61" s="3"/>
-      <c r="P61" s="3"/>
-      <c r="Q61" s="3"/>
-      <c r="R61" s="3"/>
-      <c r="S61" s="3"/>
-      <c r="T61" s="3"/>
-      <c r="U61" s="3"/>
-      <c r="V61" s="3"/>
-      <c r="W61" s="3"/>
-      <c r="X61" s="3"/>
-      <c r="Y61" s="3"/>
-      <c r="Z61" s="3"/>
-      <c r="AA61" s="3"/>
-      <c r="AB61" s="3"/>
-      <c r="AC61" s="3"/>
-      <c r="AD61" s="3"/>
-      <c r="AE61" s="3"/>
-      <c r="AF61" s="3"/>
-      <c r="AG61" s="3"/>
-      <c r="AH61" s="3"/>
+    <row r="61" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C61" s="1">
+        <v>57</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O61" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P61" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R61" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X61" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y61" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z61" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC61" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD61" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG61" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH61" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="62" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
-      <c r="N62" s="3"/>
-      <c r="O62" s="3"/>
-      <c r="P62" s="3"/>
-      <c r="Q62" s="3"/>
-      <c r="R62" s="3"/>
-      <c r="S62" s="3"/>
-      <c r="T62" s="3"/>
-      <c r="U62" s="3"/>
-      <c r="V62" s="3"/>
-      <c r="W62" s="3"/>
-      <c r="X62" s="3"/>
-      <c r="Y62" s="3"/>
-      <c r="Z62" s="3"/>
-      <c r="AA62" s="3"/>
-      <c r="AB62" s="3"/>
-      <c r="AC62" s="3"/>
-      <c r="AD62" s="3"/>
-      <c r="AE62" s="3"/>
-      <c r="AF62" s="3"/>
-      <c r="AG62" s="3"/>
-      <c r="AH62" s="3"/>
+    <row r="62" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C62" s="1">
+        <v>58</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O62" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P62" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R62" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X62" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y62" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="Z62" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC62" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD62" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG62" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH62" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="63" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
-      <c r="K63" s="3"/>
-      <c r="L63" s="3"/>
-      <c r="M63" s="3"/>
-      <c r="N63" s="3"/>
-      <c r="O63" s="3"/>
-      <c r="P63" s="3"/>
-      <c r="Q63" s="3"/>
-      <c r="R63" s="3"/>
-      <c r="S63" s="3"/>
-      <c r="T63" s="3"/>
-      <c r="U63" s="3"/>
-      <c r="V63" s="3"/>
-      <c r="W63" s="3"/>
-      <c r="X63" s="3"/>
-      <c r="Y63" s="3"/>
-      <c r="Z63" s="3"/>
-      <c r="AA63" s="3"/>
-      <c r="AB63" s="3"/>
-      <c r="AC63" s="3"/>
-      <c r="AD63" s="3"/>
-      <c r="AE63" s="3"/>
-      <c r="AF63" s="3"/>
-      <c r="AG63" s="3"/>
-      <c r="AH63" s="3"/>
+    <row r="63" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C63" s="1">
+        <v>59</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O63" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P63" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q63" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="R63" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X63" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y63" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z63" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC63" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD63" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG63" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH63" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="64" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D64" s="3"/>
-      <c r="E64" s="3"/>
-      <c r="F64" s="3"/>
-      <c r="G64" s="3"/>
-      <c r="H64" s="3"/>
-      <c r="I64" s="3"/>
-      <c r="J64" s="3"/>
-      <c r="K64" s="3"/>
-      <c r="L64" s="3"/>
-      <c r="M64" s="3"/>
-      <c r="N64" s="3"/>
-      <c r="O64" s="3"/>
-      <c r="P64" s="3"/>
-      <c r="Q64" s="3"/>
-      <c r="R64" s="3"/>
-      <c r="S64" s="3"/>
-      <c r="T64" s="3"/>
-      <c r="U64" s="3"/>
-      <c r="V64" s="3"/>
-      <c r="W64" s="3"/>
-      <c r="X64" s="3"/>
-      <c r="Y64" s="3"/>
-      <c r="Z64" s="3"/>
-      <c r="AA64" s="3"/>
-      <c r="AB64" s="3"/>
-      <c r="AC64" s="3"/>
-      <c r="AD64" s="3"/>
-      <c r="AE64" s="3"/>
-      <c r="AF64" s="3"/>
-      <c r="AG64" s="3"/>
-      <c r="AH64" s="3"/>
+    <row r="64" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C64" s="1">
+        <v>60</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O64" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P64" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R64" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="V64" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="W64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X64" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y64" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z64" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC64" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD64" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG64" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH64" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="65" spans="4:34" x14ac:dyDescent="0.25">
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="3"/>
-      <c r="J65" s="3"/>
-      <c r="K65" s="3"/>
-      <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
-      <c r="N65" s="3"/>
-      <c r="O65" s="3"/>
-      <c r="P65" s="3"/>
-      <c r="Q65" s="3"/>
-      <c r="R65" s="3"/>
-      <c r="S65" s="3"/>
-      <c r="T65" s="3"/>
-      <c r="U65" s="3"/>
-      <c r="V65" s="3"/>
-      <c r="W65" s="3"/>
-      <c r="X65" s="3"/>
-      <c r="Y65" s="3"/>
-      <c r="Z65" s="3"/>
-      <c r="AA65" s="3"/>
-      <c r="AB65" s="3"/>
-      <c r="AC65" s="3"/>
-      <c r="AD65" s="3"/>
-      <c r="AE65" s="3"/>
-      <c r="AF65" s="3"/>
-      <c r="AG65" s="3"/>
-      <c r="AH65" s="3"/>
+    <row r="65" spans="2:34" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="M65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="N65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="O65" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="P65" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="R65" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="S65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="T65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="U65" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="V65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="W65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="X65" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Y65" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z65" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC65" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="AD65" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="AE65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AG65" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="AH65" s="3" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="66" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D66" s="3"/>
       <c r="E66" s="3"/>
       <c r="F66" s="3"/>
@@ -5609,7 +7431,7 @@
       <c r="AG66" s="3"/>
       <c r="AH66" s="3"/>
     </row>
-    <row r="67" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D67" s="3"/>
       <c r="E67" s="3"/>
       <c r="F67" s="3"/>
@@ -5642,7 +7464,7 @@
       <c r="AG67" s="3"/>
       <c r="AH67" s="3"/>
     </row>
-    <row r="68" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D68" s="3"/>
       <c r="E68" s="3"/>
       <c r="F68" s="3"/>
@@ -5675,7 +7497,7 @@
       <c r="AG68" s="3"/>
       <c r="AH68" s="3"/>
     </row>
-    <row r="69" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D69" s="3"/>
       <c r="E69" s="3"/>
       <c r="F69" s="3"/>
@@ -5708,7 +7530,7 @@
       <c r="AG69" s="3"/>
       <c r="AH69" s="3"/>
     </row>
-    <row r="70" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D70" s="3"/>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
@@ -5741,7 +7563,7 @@
       <c r="AG70" s="3"/>
       <c r="AH70" s="3"/>
     </row>
-    <row r="71" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D71" s="3"/>
       <c r="E71" s="3"/>
       <c r="F71" s="3"/>
@@ -5774,7 +7596,7 @@
       <c r="AG71" s="3"/>
       <c r="AH71" s="3"/>
     </row>
-    <row r="72" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D72" s="3"/>
       <c r="E72" s="3"/>
       <c r="F72" s="3"/>
@@ -5807,7 +7629,7 @@
       <c r="AG72" s="3"/>
       <c r="AH72" s="3"/>
     </row>
-    <row r="73" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D73" s="3"/>
       <c r="E73" s="3"/>
       <c r="F73" s="3"/>
@@ -5840,7 +7662,7 @@
       <c r="AG73" s="3"/>
       <c r="AH73" s="3"/>
     </row>
-    <row r="74" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D74" s="3"/>
       <c r="E74" s="3"/>
       <c r="F74" s="3"/>
@@ -5873,7 +7695,7 @@
       <c r="AG74" s="3"/>
       <c r="AH74" s="3"/>
     </row>
-    <row r="75" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D75" s="3"/>
       <c r="E75" s="3"/>
       <c r="F75" s="3"/>
@@ -5906,7 +7728,7 @@
       <c r="AG75" s="3"/>
       <c r="AH75" s="3"/>
     </row>
-    <row r="76" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D76" s="3"/>
       <c r="E76" s="3"/>
       <c r="F76" s="3"/>
@@ -5939,7 +7761,7 @@
       <c r="AG76" s="3"/>
       <c r="AH76" s="3"/>
     </row>
-    <row r="77" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D77" s="3"/>
       <c r="E77" s="3"/>
       <c r="F77" s="3"/>
@@ -5972,7 +7794,7 @@
       <c r="AG77" s="3"/>
       <c r="AH77" s="3"/>
     </row>
-    <row r="78" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D78" s="3"/>
       <c r="E78" s="3"/>
       <c r="F78" s="3"/>
@@ -6005,7 +7827,7 @@
       <c r="AG78" s="3"/>
       <c r="AH78" s="3"/>
     </row>
-    <row r="79" spans="4:34" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:34" x14ac:dyDescent="0.25">
       <c r="D79" s="3"/>
       <c r="E79" s="3"/>
       <c r="F79" s="3"/>

</xml_diff>

<commit_message>
Added read instruction priv in state table
</commit_message>
<xml_diff>
--- a/StateTable/StateTable.xlsx
+++ b/StateTable/StateTable.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Edwin\Sparc\icom4215-sparc-project\StateTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\Code\repos\icom4215-sparc-project\StateTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5047" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5353" uniqueCount="358">
   <si>
     <t>PC_Enable</t>
   </si>
@@ -984,9 +984,6 @@
     <t>MDR disable, store value</t>
   </si>
   <si>
-    <t>swap</t>
-  </si>
-  <si>
     <t>Get PC in Alu</t>
   </si>
   <si>
@@ -1057,6 +1054,51 @@
   </si>
   <si>
     <t>NPC disable</t>
+  </si>
+  <si>
+    <t>RDWIM</t>
+  </si>
+  <si>
+    <t>4'b1000</t>
+  </si>
+  <si>
+    <t>Enable reg</t>
+  </si>
+  <si>
+    <t>Disable</t>
+  </si>
+  <si>
+    <t>Check S</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>S = 1  (Go to trap #5)</t>
+  </si>
+  <si>
+    <t>(S = 0) Init MuxB</t>
+  </si>
+  <si>
+    <t>RDTBR</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>116</t>
+  </si>
+  <si>
+    <t>117</t>
+  </si>
+  <si>
+    <t>4'b1001</t>
+  </si>
+  <si>
+    <t>RDPSR</t>
+  </si>
+  <si>
+    <t>4'b1010</t>
   </si>
 </sst>
 </file>
@@ -1072,7 +1114,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1082,6 +1124,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1098,7 +1146,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1131,6 +1179,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1465,41 +1519,41 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
-      <c r="AD2" s="11" t="s">
+      <c r="AD2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
     </row>
     <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -8485,13 +8539,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH124"/>
+  <dimension ref="A1:AH126"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8530,41 +8584,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11" t="s">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -8616,7 +8670,7 @@
         <v>7</v>
       </c>
       <c r="Q2" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>153</v>
@@ -8675,7 +8729,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>27</v>
@@ -8761,7 +8815,7 @@
     </row>
     <row r="4" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C4" s="7" t="s">
         <v>31</v>
@@ -8894,7 +8948,7 @@
     </row>
     <row r="6" spans="1:34" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C6" s="10" t="s">
         <v>81</v>
@@ -8920,7 +8974,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="C7" s="10" t="s">
         <v>82</v>
@@ -9003,7 +9057,7 @@
     </row>
     <row r="8" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>83</v>
@@ -9079,7 +9133,7 @@
         <v>27</v>
       </c>
       <c r="AB8" s="6" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="AC8" s="7" t="s">
         <v>27</v>
@@ -9087,7 +9141,7 @@
     </row>
     <row r="9" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>84</v>
@@ -9171,7 +9225,7 @@
     </row>
     <row r="10" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C10" s="10" t="s">
         <v>85</v>
@@ -9255,7 +9309,7 @@
     </row>
     <row r="11" spans="1:34" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C11" s="10" t="s">
         <v>86</v>
@@ -10012,7 +10066,7 @@
     </row>
     <row r="20" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>93</v>
@@ -10347,7 +10401,7 @@
     </row>
     <row r="24" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>97</v>
@@ -10848,7 +10902,7 @@
     </row>
     <row r="30" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B30" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>193</v>
@@ -11014,7 +11068,7 @@
     </row>
     <row r="32" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>154</v>
@@ -11432,7 +11486,7 @@
     </row>
     <row r="37" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>192</v>
@@ -11601,7 +11655,7 @@
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B39" s="4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>205</v>
@@ -11933,7 +11987,7 @@
     </row>
     <row r="43" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>154</v>
@@ -12102,7 +12156,7 @@
     </row>
     <row r="45" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B45" s="4" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C45" s="10" t="s">
         <v>210</v>
@@ -12147,10 +12201,10 @@
         <v>27</v>
       </c>
       <c r="R45" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="S45" s="6" t="s">
         <v>339</v>
-      </c>
-      <c r="S45" s="6" t="s">
-        <v>340</v>
       </c>
       <c r="T45" s="4" t="s">
         <v>27</v>
@@ -14962,7 +15016,7 @@
         <v>151</v>
       </c>
       <c r="C80" s="10" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>27</v>
@@ -15045,7 +15099,7 @@
         <v>260</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>27</v>
@@ -16349,6 +16403,9 @@
       <c r="P96" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q96" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R96" s="5" t="s">
         <v>27</v>
       </c>
@@ -16432,6 +16489,9 @@
       <c r="P97" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q97" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R97" s="5" t="s">
         <v>27</v>
       </c>
@@ -16515,6 +16575,9 @@
       <c r="P98" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q98" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R98" s="5" t="s">
         <v>27</v>
       </c>
@@ -16598,6 +16661,9 @@
       <c r="P99" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q99" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R99" s="5" t="s">
         <v>27</v>
       </c>
@@ -16681,6 +16747,9 @@
       <c r="P100" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q100" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R100" s="5" t="s">
         <v>27</v>
       </c>
@@ -16764,6 +16833,9 @@
       <c r="P101" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q101" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R101" s="5" t="s">
         <v>27</v>
       </c>
@@ -16850,6 +16922,9 @@
       <c r="P102" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q102" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R102" s="5" t="s">
         <v>27</v>
       </c>
@@ -16936,6 +17011,9 @@
       <c r="P103" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q103" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R103" s="6" t="s">
         <v>183</v>
       </c>
@@ -17019,6 +17097,9 @@
       <c r="P104" s="6" t="s">
         <v>183</v>
       </c>
+      <c r="Q104" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R104" s="5" t="s">
         <v>27</v>
       </c>
@@ -17102,6 +17183,9 @@
       <c r="P105" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q105" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R105" s="5" t="s">
         <v>27</v>
       </c>
@@ -17185,6 +17269,9 @@
       <c r="P106" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q106" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R106" s="5" t="s">
         <v>27</v>
       </c>
@@ -17224,7 +17311,7 @@
     </row>
     <row r="107" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B107" s="4" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>309</v>
@@ -17266,6 +17353,9 @@
         <v>27</v>
       </c>
       <c r="P107" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q107" s="11" t="s">
         <v>27</v>
       </c>
       <c r="R107" s="5" t="s">
@@ -17351,6 +17441,9 @@
       <c r="P108" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q108" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R108" s="5" t="s">
         <v>27</v>
       </c>
@@ -17434,6 +17527,9 @@
       <c r="P109" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q109" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R109" s="5" t="s">
         <v>27</v>
       </c>
@@ -17473,7 +17569,7 @@
     </row>
     <row r="110" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B110" s="4" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>312</v>
@@ -17517,6 +17613,9 @@
       <c r="P110" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q110" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R110" s="5" t="s">
         <v>27</v>
       </c>
@@ -17556,218 +17655,233 @@
     </row>
     <row r="111" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A111" s="4" t="s">
-        <v>319</v>
+        <v>343</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>245</v>
-      </c>
-      <c r="C111" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="C111" s="11" t="s">
         <v>313</v>
       </c>
-      <c r="D111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="R111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="T111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="U111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="X111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB111" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC111" s="5" t="s">
+      <c r="D111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB111" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC111" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="112" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="C112" s="10" t="s">
+      <c r="B112" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C112" s="11" t="s">
         <v>314</v>
       </c>
-      <c r="D112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="R112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="T112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="U112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="X112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB112" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC112" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="113" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C113" s="10" t="s">
+      <c r="D112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB112" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC112" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="113" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B113" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="C113" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="D113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="J113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O113" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P113" s="5" t="s">
+      <c r="D113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P113" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q113" s="11" t="s">
         <v>27</v>
       </c>
       <c r="R113" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="S113" s="5" t="s">
-        <v>27</v>
+      <c r="S113" s="6" t="s">
+        <v>344</v>
       </c>
       <c r="T113" s="5" t="s">
         <v>27</v>
@@ -17784,14 +17898,14 @@
       <c r="X113" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Y113" s="5" t="s">
+      <c r="Y113" s="6" t="s">
         <v>27</v>
       </c>
       <c r="Z113" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AA113" s="5" t="s">
-        <v>27</v>
+      <c r="AA113" s="6" t="s">
+        <v>166</v>
       </c>
       <c r="AB113" s="5" t="s">
         <v>27</v>
@@ -17800,8 +17914,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="114" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C114" s="10" t="s">
+    <row r="114" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B114" s="4" t="s">
+        <v>345</v>
+      </c>
+      <c r="C114" s="11" t="s">
         <v>134</v>
       </c>
       <c r="D114" s="5" t="s">
@@ -17819,8 +17936,8 @@
       <c r="H114" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I114" s="5" t="s">
-        <v>27</v>
+      <c r="I114" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="J114" s="5" t="s">
         <v>27</v>
@@ -17843,6 +17960,9 @@
       <c r="P114" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q114" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R114" s="5" t="s">
         <v>27</v>
       </c>
@@ -17880,8 +18000,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="115" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C115" s="10" t="s">
+    <row r="115" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B115" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C115" s="11" t="s">
         <v>315</v>
       </c>
       <c r="D115" s="5" t="s">
@@ -17899,7 +18022,7 @@
       <c r="H115" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="I115" s="5" t="s">
+      <c r="I115" s="6" t="s">
         <v>27</v>
       </c>
       <c r="J115" s="5" t="s">
@@ -17923,6 +18046,9 @@
       <c r="P115" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q115" s="11" t="s">
+        <v>27</v>
+      </c>
       <c r="R115" s="5" t="s">
         <v>27</v>
       </c>
@@ -17960,234 +18086,880 @@
         <v>27</v>
       </c>
     </row>
-    <row r="116" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C116" s="10" t="s">
+    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A116" s="4" t="s">
+        <v>351</v>
+      </c>
+      <c r="B116" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="C116" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="D116" s="5"/>
-      <c r="E116" s="5"/>
-      <c r="F116" s="5"/>
-      <c r="G116" s="5"/>
-      <c r="H116" s="5"/>
-      <c r="I116" s="5"/>
-      <c r="J116" s="5"/>
-      <c r="K116" s="5"/>
-      <c r="L116" s="5"/>
-      <c r="M116" s="5"/>
-      <c r="N116" s="5"/>
-      <c r="O116" s="5"/>
-      <c r="P116" s="5"/>
-      <c r="R116" s="5"/>
-      <c r="S116" s="5"/>
-      <c r="T116" s="5"/>
-      <c r="U116" s="5"/>
-      <c r="V116" s="5"/>
-      <c r="W116" s="5"/>
-      <c r="X116" s="5"/>
-      <c r="Y116" s="5"/>
-      <c r="Z116" s="5"/>
-      <c r="AA116" s="5"/>
-      <c r="AB116" s="5"/>
-      <c r="AC116" s="5"/>
-    </row>
-    <row r="117" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C117" s="8"/>
-      <c r="D117" s="5"/>
-      <c r="E117" s="5"/>
-      <c r="F117" s="5"/>
-      <c r="G117" s="5"/>
-      <c r="H117" s="5"/>
-      <c r="I117" s="5"/>
-      <c r="J117" s="5"/>
-      <c r="K117" s="5"/>
-      <c r="L117" s="5"/>
-      <c r="M117" s="5"/>
-      <c r="N117" s="5"/>
-      <c r="O117" s="5"/>
-      <c r="P117" s="5"/>
-      <c r="R117" s="5"/>
-      <c r="S117" s="5"/>
-      <c r="T117" s="5"/>
-      <c r="U117" s="5"/>
-      <c r="V117" s="5"/>
-      <c r="W117" s="5"/>
-      <c r="X117" s="5"/>
-      <c r="Y117" s="5"/>
-      <c r="Z117" s="5"/>
-      <c r="AA117" s="5"/>
-      <c r="AB117" s="5"/>
-      <c r="AC117" s="5"/>
-    </row>
-    <row r="118" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-      <c r="E118" s="5"/>
-      <c r="F118" s="5"/>
-      <c r="G118" s="5"/>
-      <c r="H118" s="5"/>
-      <c r="I118" s="5"/>
-      <c r="J118" s="5"/>
-      <c r="K118" s="5"/>
-      <c r="L118" s="5"/>
-      <c r="M118" s="5"/>
-      <c r="N118" s="5"/>
-      <c r="O118" s="5"/>
-      <c r="P118" s="5"/>
-      <c r="R118" s="5"/>
-      <c r="S118" s="5"/>
-      <c r="T118" s="5"/>
-      <c r="U118" s="5"/>
-      <c r="V118" s="5"/>
-      <c r="W118" s="5"/>
-      <c r="X118" s="5"/>
-      <c r="Y118" s="5"/>
-      <c r="Z118" s="5"/>
-      <c r="AA118" s="5"/>
-      <c r="AB118" s="5"/>
-      <c r="AC118" s="5"/>
-    </row>
-    <row r="119" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
-      <c r="E119" s="5"/>
-      <c r="F119" s="5"/>
-      <c r="G119" s="5"/>
-      <c r="H119" s="5"/>
-      <c r="I119" s="5"/>
-      <c r="J119" s="5"/>
-      <c r="K119" s="5"/>
-      <c r="L119" s="5"/>
-      <c r="M119" s="5"/>
-      <c r="N119" s="5"/>
-      <c r="O119" s="5"/>
-      <c r="P119" s="5"/>
-      <c r="R119" s="5"/>
-      <c r="S119" s="5"/>
-      <c r="T119" s="5"/>
-      <c r="U119" s="5"/>
-      <c r="V119" s="5"/>
-      <c r="W119" s="5"/>
-      <c r="X119" s="5"/>
-      <c r="Y119" s="5"/>
-      <c r="Z119" s="5"/>
-      <c r="AA119" s="5"/>
-      <c r="AB119" s="5"/>
-      <c r="AC119" s="5"/>
-    </row>
-    <row r="120" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
-      <c r="E120" s="5"/>
-      <c r="F120" s="5"/>
-      <c r="G120" s="5"/>
-      <c r="H120" s="5"/>
-      <c r="I120" s="5"/>
-      <c r="J120" s="5"/>
-      <c r="K120" s="5"/>
-      <c r="L120" s="5"/>
-      <c r="M120" s="5"/>
-      <c r="N120" s="5"/>
-      <c r="O120" s="5"/>
-      <c r="P120" s="5"/>
-      <c r="R120" s="5"/>
-      <c r="S120" s="5"/>
-      <c r="T120" s="5"/>
-      <c r="U120" s="5"/>
-      <c r="V120" s="5"/>
-      <c r="W120" s="5"/>
-      <c r="X120" s="5"/>
-      <c r="Y120" s="5"/>
-      <c r="Z120" s="5"/>
-      <c r="AA120" s="5"/>
-      <c r="AB120" s="5"/>
-      <c r="AC120" s="5"/>
-    </row>
-    <row r="121" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C121" s="5"/>
-      <c r="D121" s="5"/>
-      <c r="E121" s="5"/>
-      <c r="F121" s="5"/>
-      <c r="G121" s="5"/>
-      <c r="H121" s="5"/>
-      <c r="I121" s="5"/>
-      <c r="J121" s="5"/>
-      <c r="K121" s="5"/>
-      <c r="L121" s="5"/>
-      <c r="M121" s="5"/>
-      <c r="N121" s="5"/>
-      <c r="O121" s="5"/>
-      <c r="P121" s="5"/>
-      <c r="R121" s="5"/>
-      <c r="S121" s="5"/>
-      <c r="T121" s="5"/>
-      <c r="U121" s="5"/>
-      <c r="V121" s="5"/>
-      <c r="W121" s="5"/>
-      <c r="X121" s="5"/>
-      <c r="Y121" s="5"/>
-      <c r="Z121" s="5"/>
-      <c r="AA121" s="5"/>
-      <c r="AB121" s="5"/>
-      <c r="AC121" s="5"/>
-    </row>
-    <row r="122" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C122" s="5"/>
-      <c r="D122" s="5"/>
-      <c r="E122" s="5"/>
-      <c r="F122" s="5"/>
-      <c r="G122" s="5"/>
-      <c r="H122" s="5"/>
-      <c r="I122" s="5"/>
-      <c r="J122" s="5"/>
-      <c r="K122" s="5"/>
-      <c r="L122" s="5"/>
-      <c r="M122" s="5"/>
-      <c r="N122" s="5"/>
-      <c r="O122" s="5"/>
-      <c r="P122" s="5"/>
-      <c r="R122" s="5"/>
-      <c r="S122" s="5"/>
-      <c r="T122" s="5"/>
-      <c r="U122" s="5"/>
-      <c r="V122" s="5"/>
-      <c r="W122" s="5"/>
-      <c r="X122" s="5"/>
-      <c r="Y122" s="5"/>
-      <c r="Z122" s="5"/>
-      <c r="AA122" s="5"/>
-      <c r="AB122" s="5"/>
-      <c r="AC122" s="5"/>
-    </row>
-    <row r="123" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
-      <c r="E123" s="5"/>
-      <c r="F123" s="5"/>
-      <c r="G123" s="5"/>
-      <c r="H123" s="5"/>
-      <c r="I123" s="5"/>
-      <c r="J123" s="5"/>
-      <c r="K123" s="5"/>
-      <c r="L123" s="5"/>
-      <c r="M123" s="5"/>
-      <c r="N123" s="5"/>
-      <c r="O123" s="5"/>
-      <c r="P123" s="5"/>
-      <c r="R123" s="5"/>
-      <c r="S123" s="5"/>
-      <c r="T123" s="5"/>
-      <c r="U123" s="5"/>
-      <c r="V123" s="5"/>
-      <c r="W123" s="5"/>
-      <c r="X123" s="5"/>
-      <c r="Y123" s="5"/>
-      <c r="Z123" s="5"/>
-      <c r="AA123" s="5"/>
-      <c r="AB123" s="5"/>
-      <c r="AC123" s="5"/>
-    </row>
-    <row r="124" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C124" s="5"/>
+      <c r="D116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC116" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B117" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C117" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="D117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC117" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="118" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B118" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="C118" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="D118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S118" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="T118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y118" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA118" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC118" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B119" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="C119" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="D119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC119" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B120" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C120" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I120" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC120" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="121" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A121" s="11" t="s">
+        <v>356</v>
+      </c>
+      <c r="B121" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="C121" s="11" t="s">
+        <v>316</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC121" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="122" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A122" s="11"/>
+      <c r="B122" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C122" s="11" t="s">
+        <v>348</v>
+      </c>
+      <c r="D122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB122" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC122" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="123" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A123" s="11"/>
+      <c r="B123" s="11" t="s">
+        <v>350</v>
+      </c>
+      <c r="C123" s="11" t="s">
+        <v>352</v>
+      </c>
+      <c r="D123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S123" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="T123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y123" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA123" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB123" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC123" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="124" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A124" s="11"/>
+      <c r="B124" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="C124" s="11" t="s">
+        <v>353</v>
+      </c>
+      <c r="D124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I124" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB124" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC124" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="125" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A125" s="11"/>
+      <c r="B125" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C125" s="11" t="s">
+        <v>354</v>
+      </c>
+      <c r="D125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I125" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="R125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB125" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC125" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="126" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A126" s="4" t="s">
+        <v>244</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
idk wat is dis commit
</commit_message>
<xml_diff>
--- a/StateTable/StateTable.xlsx
+++ b/StateTable/StateTable.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5353" uniqueCount="358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5530" uniqueCount="367">
   <si>
     <t>PC_Enable</t>
   </si>
@@ -1074,9 +1074,6 @@
     <t>114</t>
   </si>
   <si>
-    <t>S = 1  (Go to trap #5)</t>
-  </si>
-  <si>
     <t>(S = 0) Init MuxB</t>
   </si>
   <si>
@@ -1099,6 +1096,36 @@
   </si>
   <si>
     <t>4'b1010</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>119</t>
+  </si>
+  <si>
+    <t>120</t>
+  </si>
+  <si>
+    <t>121</t>
+  </si>
+  <si>
+    <t>122</t>
+  </si>
+  <si>
+    <t>123</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>6'b000011</t>
+  </si>
+  <si>
+    <t>TBR enable</t>
+  </si>
+  <si>
+    <t>TBR Disable</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1124,12 +1151,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1184,7 +1205,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1470,10 +1491,10 @@
   <dimension ref="A2:AL79"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="A2:AH65"/>
+      <selection pane="bottomRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1519,41 +1540,41 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="H2" s="13"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="13"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
+      <c r="U2" s="13"/>
+      <c r="V2" s="13"/>
+      <c r="W2" s="13"/>
+      <c r="X2" s="13"/>
+      <c r="Y2" s="13"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
-      <c r="AD2" s="12" t="s">
+      <c r="AD2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13"/>
     </row>
     <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -8539,13 +8560,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH126"/>
+  <dimension ref="A1:AH181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C105" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="P3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B126" sqref="B126"/>
+      <selection pane="bottomRight" activeCell="Q120" sqref="Q120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8566,7 +8587,7 @@
     <col min="15" max="15" width="13.85546875" style="4" customWidth="1"/>
     <col min="16" max="16" width="16" style="4" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" style="9" customWidth="1"/>
-    <col min="18" max="18" width="16" style="4" customWidth="1"/>
+    <col min="18" max="18" width="19.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="17.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
@@ -8584,41 +8605,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" x14ac:dyDescent="0.25">
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12" t="s">
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
+      <c r="AE1" s="13"/>
+      <c r="AF1" s="13"/>
+      <c r="AG1" s="13"/>
+      <c r="AH1" s="13"/>
     </row>
     <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -8943,6 +8964,9 @@
         <v>27</v>
       </c>
       <c r="P5" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q5" s="12" t="s">
         <v>27</v>
       </c>
     </row>
@@ -8968,6 +8992,9 @@
       <c r="N6" s="10"/>
       <c r="O6" s="10"/>
       <c r="P6" s="10"/>
+      <c r="Q6" s="12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
@@ -9018,6 +9045,9 @@
       <c r="P7" s="7" t="s">
         <v>27</v>
       </c>
+      <c r="Q7" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R7" s="6" t="s">
         <v>183</v>
       </c>
@@ -9101,7 +9131,9 @@
       <c r="P8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Q8" s="9"/>
+      <c r="Q8" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R8" s="7" t="s">
         <v>27</v>
       </c>
@@ -9185,7 +9217,9 @@
       <c r="P9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Q9" s="9"/>
+      <c r="Q9" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R9" s="7" t="s">
         <v>27</v>
       </c>
@@ -9269,7 +9303,9 @@
       <c r="P10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Q10" s="9"/>
+      <c r="Q10" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R10" s="7" t="s">
         <v>27</v>
       </c>
@@ -9353,7 +9389,9 @@
       <c r="P11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="Q11" s="9"/>
+      <c r="Q11" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R11" s="7" t="s">
         <v>27</v>
       </c>
@@ -9440,6 +9478,9 @@
       <c r="P12" s="6" t="s">
         <v>170</v>
       </c>
+      <c r="Q12" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R12" s="6" t="s">
         <v>168</v>
       </c>
@@ -9523,6 +9564,9 @@
       <c r="P13" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q13" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R13" s="4" t="s">
         <v>27</v>
       </c>
@@ -9606,6 +9650,9 @@
       <c r="P14" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q14" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R14" s="4" t="s">
         <v>27</v>
       </c>
@@ -9692,6 +9739,9 @@
       <c r="P15" s="9" t="s">
         <v>27</v>
       </c>
+      <c r="Q15" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R15" s="4" t="s">
         <v>27</v>
       </c>
@@ -9778,6 +9828,9 @@
       <c r="P16" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q16" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R16" s="6" t="s">
         <v>172</v>
       </c>
@@ -9861,6 +9914,9 @@
       <c r="P17" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q17" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R17" s="4" t="s">
         <v>27</v>
       </c>
@@ -9944,6 +10000,9 @@
       <c r="P18" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q18" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R18" s="4" t="s">
         <v>27</v>
       </c>
@@ -10027,6 +10086,9 @@
       <c r="P19" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q19" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R19" s="4" t="s">
         <v>27</v>
       </c>
@@ -10110,6 +10172,9 @@
       <c r="P20" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q20" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R20" s="6" t="s">
         <v>179</v>
       </c>
@@ -10193,6 +10258,9 @@
       <c r="P21" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q21" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R21" s="4" t="s">
         <v>27</v>
       </c>
@@ -10279,6 +10347,9 @@
       <c r="P22" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q22" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R22" s="4" t="s">
         <v>27</v>
       </c>
@@ -10362,6 +10433,9 @@
       <c r="P23" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q23" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R23" s="4" t="s">
         <v>27</v>
       </c>
@@ -10445,6 +10519,9 @@
       <c r="P24" s="6" t="s">
         <v>185</v>
       </c>
+      <c r="Q24" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R24" s="6" t="s">
         <v>186</v>
       </c>
@@ -10528,6 +10605,9 @@
       <c r="P25" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q25" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R25" s="4" t="s">
         <v>27</v>
       </c>
@@ -10611,6 +10691,9 @@
       <c r="P26" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q26" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R26" s="4" t="s">
         <v>27</v>
       </c>
@@ -10697,6 +10780,9 @@
       <c r="P27" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q27" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R27" s="6" t="s">
         <v>179</v>
       </c>
@@ -10780,6 +10866,9 @@
       <c r="P28" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q28" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R28" s="4" t="s">
         <v>27</v>
       </c>
@@ -10863,6 +10952,9 @@
       <c r="P29" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q29" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R29" s="4" t="s">
         <v>27</v>
       </c>
@@ -10946,6 +11038,9 @@
       <c r="P30" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q30" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R30" s="6" t="s">
         <v>179</v>
       </c>
@@ -11029,6 +11124,9 @@
       <c r="P31" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q31" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R31" s="4" t="s">
         <v>27</v>
       </c>
@@ -11115,6 +11213,9 @@
       <c r="P32" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q32" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R32" s="4" t="s">
         <v>27</v>
       </c>
@@ -11198,6 +11299,9 @@
       <c r="P33" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q33" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R33" s="4" t="s">
         <v>27</v>
       </c>
@@ -11281,6 +11385,9 @@
       <c r="P34" s="6" t="s">
         <v>185</v>
       </c>
+      <c r="Q34" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R34" s="6" t="s">
         <v>186</v>
       </c>
@@ -11364,6 +11471,9 @@
       <c r="P35" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q35" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R35" s="4" t="s">
         <v>27</v>
       </c>
@@ -11447,6 +11557,9 @@
       <c r="P36" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q36" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R36" s="4" t="s">
         <v>27</v>
       </c>
@@ -11533,6 +11646,9 @@
       <c r="P37" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q37" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R37" s="6" t="s">
         <v>172</v>
       </c>
@@ -11616,6 +11732,9 @@
       <c r="P38" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q38" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R38" s="4" t="s">
         <v>27</v>
       </c>
@@ -11699,6 +11818,9 @@
       <c r="P39" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q39" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R39" s="4" t="s">
         <v>27</v>
       </c>
@@ -11782,6 +11904,9 @@
       <c r="P40" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q40" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R40" s="4" t="s">
         <v>27</v>
       </c>
@@ -11865,6 +11990,9 @@
       <c r="P41" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q41" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R41" s="4" t="s">
         <v>27</v>
       </c>
@@ -11948,6 +12076,9 @@
       <c r="P42" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q42" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R42" s="4" t="s">
         <v>27</v>
       </c>
@@ -12034,6 +12165,9 @@
       <c r="P43" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q43" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R43" s="4" t="s">
         <v>27</v>
       </c>
@@ -12117,6 +12251,9 @@
       <c r="P44" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q44" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R44" s="4" t="s">
         <v>27</v>
       </c>
@@ -12200,6 +12337,9 @@
       <c r="P45" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q45" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R45" s="6" t="s">
         <v>338</v>
       </c>
@@ -12283,6 +12423,9 @@
       <c r="P46" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q46" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R46" s="4" t="s">
         <v>27</v>
       </c>
@@ -12366,6 +12509,9 @@
       <c r="P47" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q47" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R47" s="4" t="s">
         <v>27</v>
       </c>
@@ -12452,6 +12598,9 @@
       <c r="P48" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q48" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R48" s="6" t="s">
         <v>183</v>
       </c>
@@ -12535,6 +12684,9 @@
       <c r="P49" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q49" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R49" s="4" t="s">
         <v>27</v>
       </c>
@@ -12618,6 +12770,9 @@
       <c r="P50" s="6" t="s">
         <v>222</v>
       </c>
+      <c r="Q50" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R50" s="6" t="s">
         <v>183</v>
       </c>
@@ -12701,6 +12856,9 @@
       <c r="P51" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q51" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R51" s="4" t="s">
         <v>27</v>
       </c>
@@ -12784,6 +12942,9 @@
       <c r="P52" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q52" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R52" s="4" t="s">
         <v>27</v>
       </c>
@@ -12870,6 +13031,9 @@
       <c r="P53" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q53" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R53" s="6" t="s">
         <v>168</v>
       </c>
@@ -12953,6 +13117,9 @@
       <c r="P54" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q54" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R54" s="4" t="s">
         <v>27</v>
       </c>
@@ -13036,6 +13203,9 @@
       <c r="P55" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q55" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R55" s="4" t="s">
         <v>27</v>
       </c>
@@ -13119,6 +13289,9 @@
       <c r="P56" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q56" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R56" s="4" t="s">
         <v>27</v>
       </c>
@@ -13202,6 +13375,9 @@
       <c r="P57" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q57" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R57" s="4" t="s">
         <v>27</v>
       </c>
@@ -13285,6 +13461,9 @@
       <c r="P58" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q58" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R58" s="4" t="s">
         <v>27</v>
       </c>
@@ -13371,6 +13550,9 @@
       <c r="P59" s="6" t="s">
         <v>183</v>
       </c>
+      <c r="Q59" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R59" s="4" t="s">
         <v>27</v>
       </c>
@@ -13457,6 +13639,9 @@
       <c r="P60" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q60" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R60" s="4" t="s">
         <v>27</v>
       </c>
@@ -13540,6 +13725,9 @@
       <c r="P61" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q61" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R61" s="4" t="s">
         <v>27</v>
       </c>
@@ -13623,6 +13811,9 @@
       <c r="P62" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q62" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R62" s="4" t="s">
         <v>27</v>
       </c>
@@ -13670,6 +13861,9 @@
       <c r="C63" s="10" t="s">
         <v>243</v>
       </c>
+      <c r="Q63" s="12" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="64" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
@@ -13720,6 +13914,9 @@
       <c r="P64" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q64" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R64" s="6" t="s">
         <v>183</v>
       </c>
@@ -13806,6 +14003,9 @@
       <c r="P65" s="6" t="s">
         <v>183</v>
       </c>
+      <c r="Q65" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R65" s="4" t="s">
         <v>27</v>
       </c>
@@ -13892,6 +14092,9 @@
       <c r="P66" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q66" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R66" s="4" t="s">
         <v>27</v>
       </c>
@@ -13975,6 +14178,9 @@
       <c r="P67" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q67" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R67" s="4" t="s">
         <v>27</v>
       </c>
@@ -14058,6 +14264,9 @@
       <c r="P68" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q68" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R68" s="4" t="s">
         <v>27</v>
       </c>
@@ -14141,6 +14350,9 @@
       <c r="P69" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q69" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R69" s="6" t="s">
         <v>222</v>
       </c>
@@ -14224,6 +14436,9 @@
       <c r="P70" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q70" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R70" s="4" t="s">
         <v>27</v>
       </c>
@@ -14307,6 +14522,9 @@
       <c r="P71" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q71" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R71" s="6" t="s">
         <v>183</v>
       </c>
@@ -14390,6 +14608,9 @@
       <c r="P72" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q72" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R72" s="4" t="s">
         <v>27</v>
       </c>
@@ -14473,6 +14694,9 @@
       <c r="P73" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q73" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R73" s="4" t="s">
         <v>27</v>
       </c>
@@ -14559,6 +14783,9 @@
       <c r="P74" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q74" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R74" s="6" t="s">
         <v>183</v>
       </c>
@@ -14642,6 +14869,9 @@
       <c r="P75" s="6" t="s">
         <v>183</v>
       </c>
+      <c r="Q75" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R75" s="4" t="s">
         <v>27</v>
       </c>
@@ -14725,6 +14955,9 @@
       <c r="P76" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q76" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R76" s="4" t="s">
         <v>27</v>
       </c>
@@ -14808,6 +15041,9 @@
       <c r="P77" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q77" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R77" s="4" t="s">
         <v>27</v>
       </c>
@@ -14891,6 +15127,9 @@
       <c r="P78" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q78" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R78" s="4" t="s">
         <v>27</v>
       </c>
@@ -14974,6 +15213,9 @@
       <c r="P79" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q79" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R79" s="6" t="s">
         <v>222</v>
       </c>
@@ -15057,6 +15299,9 @@
       <c r="P80" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q80" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R80" s="4" t="s">
         <v>27</v>
       </c>
@@ -15140,6 +15385,9 @@
       <c r="P81" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q81" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R81" s="6" t="s">
         <v>183</v>
       </c>
@@ -15223,6 +15471,9 @@
       <c r="P82" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q82" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R82" s="4" t="s">
         <v>27</v>
       </c>
@@ -15306,6 +15557,9 @@
       <c r="P83" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q83" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R83" s="4" t="s">
         <v>27</v>
       </c>
@@ -15392,6 +15646,9 @@
       <c r="P84" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q84" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R84" s="6" t="s">
         <v>183</v>
       </c>
@@ -15478,6 +15735,9 @@
       <c r="P85" s="6" t="s">
         <v>183</v>
       </c>
+      <c r="Q85" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R85" s="4" t="s">
         <v>27</v>
       </c>
@@ -15564,6 +15824,9 @@
       <c r="P86" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q86" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R86" s="4" t="s">
         <v>27</v>
       </c>
@@ -15647,6 +15910,9 @@
       <c r="P87" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q87" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R87" s="4" t="s">
         <v>27</v>
       </c>
@@ -15730,6 +15996,9 @@
       <c r="P88" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q88" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R88" s="4" t="s">
         <v>27</v>
       </c>
@@ -15816,6 +16085,9 @@
       <c r="P89" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q89" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R89" s="4" t="s">
         <v>27</v>
       </c>
@@ -15899,6 +16171,9 @@
       <c r="P90" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q90" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R90" s="4" t="s">
         <v>27</v>
       </c>
@@ -15985,6 +16260,9 @@
       <c r="P91" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q91" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R91" s="4" t="s">
         <v>27</v>
       </c>
@@ -16071,6 +16349,9 @@
       <c r="P92" s="4" t="s">
         <v>27</v>
       </c>
+      <c r="Q92" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R92" s="6" t="s">
         <v>183</v>
       </c>
@@ -16154,6 +16435,9 @@
       <c r="P93" s="6" t="s">
         <v>183</v>
       </c>
+      <c r="Q93" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R93" s="5" t="s">
         <v>27</v>
       </c>
@@ -16237,6 +16521,9 @@
       <c r="P94" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q94" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R94" s="5" t="s">
         <v>27</v>
       </c>
@@ -16320,6 +16607,9 @@
       <c r="P95" s="5" t="s">
         <v>27</v>
       </c>
+      <c r="Q95" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="R95" s="5" t="s">
         <v>27</v>
       </c>
@@ -16403,7 +16693,7 @@
       <c r="P96" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q96" s="11" t="s">
+      <c r="Q96" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R96" s="5" t="s">
@@ -16489,7 +16779,7 @@
       <c r="P97" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q97" s="11" t="s">
+      <c r="Q97" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R97" s="5" t="s">
@@ -16575,7 +16865,7 @@
       <c r="P98" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q98" s="11" t="s">
+      <c r="Q98" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R98" s="5" t="s">
@@ -16661,7 +16951,7 @@
       <c r="P99" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q99" s="11" t="s">
+      <c r="Q99" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R99" s="5" t="s">
@@ -16747,7 +17037,7 @@
       <c r="P100" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q100" s="11" t="s">
+      <c r="Q100" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R100" s="5" t="s">
@@ -16833,7 +17123,7 @@
       <c r="P101" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q101" s="11" t="s">
+      <c r="Q101" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R101" s="5" t="s">
@@ -16922,7 +17212,7 @@
       <c r="P102" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q102" s="11" t="s">
+      <c r="Q102" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R102" s="5" t="s">
@@ -17011,7 +17301,7 @@
       <c r="P103" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q103" s="11" t="s">
+      <c r="Q103" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R103" s="6" t="s">
@@ -17097,7 +17387,7 @@
       <c r="P104" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="Q104" s="11" t="s">
+      <c r="Q104" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R104" s="5" t="s">
@@ -17183,7 +17473,7 @@
       <c r="P105" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q105" s="11" t="s">
+      <c r="Q105" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R105" s="5" t="s">
@@ -17269,7 +17559,7 @@
       <c r="P106" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q106" s="11" t="s">
+      <c r="Q106" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R106" s="5" t="s">
@@ -17355,7 +17645,7 @@
       <c r="P107" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q107" s="11" t="s">
+      <c r="Q107" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R107" s="5" t="s">
@@ -17441,7 +17731,7 @@
       <c r="P108" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q108" s="11" t="s">
+      <c r="Q108" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R108" s="5" t="s">
@@ -17527,7 +17817,7 @@
       <c r="P109" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q109" s="11" t="s">
+      <c r="Q109" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R109" s="5" t="s">
@@ -17571,7 +17861,7 @@
       <c r="B110" s="4" t="s">
         <v>341</v>
       </c>
-      <c r="C110" s="10" t="s">
+      <c r="C110" s="12" t="s">
         <v>312</v>
       </c>
       <c r="D110" s="5" t="s">
@@ -17613,7 +17903,7 @@
       <c r="P110" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Q110" s="11" t="s">
+      <c r="Q110" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R110" s="5" t="s">
@@ -17660,7 +17950,7 @@
       <c r="B111" s="4" t="s">
         <v>347</v>
       </c>
-      <c r="C111" s="11" t="s">
+      <c r="C111" s="12" t="s">
         <v>313</v>
       </c>
       <c r="D111" s="11" t="s">
@@ -17702,7 +17992,7 @@
       <c r="P111" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="Q111" s="11" t="s">
+      <c r="Q111" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R111" s="11" t="s">
@@ -17743,10 +18033,10 @@
       </c>
     </row>
     <row r="112" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B112" s="13" t="s">
+      <c r="B112" s="4" t="s">
         <v>349</v>
       </c>
-      <c r="C112" s="11" t="s">
+      <c r="C112" s="12" t="s">
         <v>314</v>
       </c>
       <c r="D112" s="11" t="s">
@@ -17788,100 +18078,100 @@
       <c r="P112" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="Q112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="R112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="T112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="V112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="W112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="X112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB112" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC112" s="11" t="s">
+      <c r="Q112" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S112" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="T112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="V112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="W112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="X112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y112" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA112" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB112" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC112" s="5" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="113" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B113" s="4" t="s">
-        <v>350</v>
-      </c>
-      <c r="C113" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="C113" s="12" t="s">
         <v>125</v>
       </c>
-      <c r="D113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="N113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="O113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P113" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q113" s="11" t="s">
+      <c r="D113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I113" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P113" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q113" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R113" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="S113" s="6" t="s">
-        <v>344</v>
+      <c r="S113" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="T113" s="5" t="s">
         <v>27</v>
@@ -17898,14 +18188,14 @@
       <c r="X113" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="Y113" s="6" t="s">
+      <c r="Y113" s="5" t="s">
         <v>27</v>
       </c>
       <c r="Z113" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AA113" s="6" t="s">
-        <v>166</v>
+      <c r="AA113" s="5" t="s">
+        <v>27</v>
       </c>
       <c r="AB113" s="5" t="s">
         <v>27</v>
@@ -17916,290 +18206,290 @@
     </row>
     <row r="114" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B114" s="4" t="s">
+        <v>346</v>
+      </c>
+      <c r="C114" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I114" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="K114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="L114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="M114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="N114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="O114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="P114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q114" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="S114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="T114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="U114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="V114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="W114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="X114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB114" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC114" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="115" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A115" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B115" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="C115" s="12" t="s">
+        <v>315</v>
+      </c>
+      <c r="D115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q115" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB115" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC115" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B116" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="C116" s="12" t="s">
+        <v>316</v>
+      </c>
+      <c r="D116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q116" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S116" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="T116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y116" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA116" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB116" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC116" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="B117" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="C114" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="D114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I114" s="6" t="s">
+      <c r="C117" s="12" t="s">
+        <v>348</v>
+      </c>
+      <c r="D117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H117" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I117" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q114" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="R114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="T114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="U114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="X114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB114" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC114" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="115" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B115" s="4" t="s">
-        <v>346</v>
-      </c>
-      <c r="C115" s="11" t="s">
-        <v>315</v>
-      </c>
-      <c r="D115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="F115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="H115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I115" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="K115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="M115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="N115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="O115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="P115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q115" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="R115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="S115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="T115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="U115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="V115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="W115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="X115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB115" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC115" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="116" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A116" s="4" t="s">
-        <v>351</v>
-      </c>
-      <c r="B116" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="C116" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="D116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="N116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="O116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="R116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="T116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="V116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="W116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="X116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB116" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC116" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="117" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B117" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="C117" s="11" t="s">
-        <v>348</v>
-      </c>
-      <c r="D117" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E117" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F117" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G117" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H117" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I117" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="J117" s="11" t="s">
         <v>27</v>
       </c>
@@ -18221,7 +18511,7 @@
       <c r="P117" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="Q117" s="11" t="s">
+      <c r="Q117" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R117" s="11" t="s">
@@ -18263,290 +18553,292 @@
     </row>
     <row r="118" spans="1:29" x14ac:dyDescent="0.25">
       <c r="B118" s="11" t="s">
-        <v>350</v>
-      </c>
-      <c r="C118" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C118" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="D118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I118" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q118" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB118" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC118" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A119" s="11" t="s">
+        <v>355</v>
+      </c>
+      <c r="B119" s="11" t="s">
+        <v>347</v>
+      </c>
+      <c r="C119" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="D118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="N118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="O118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="R118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S118" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="T118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="V118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="W118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="X118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y118" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA118" s="6" t="s">
+      <c r="D119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q119" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="T119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB119" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC119" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A120" s="11"/>
+      <c r="B120" s="11" t="s">
+        <v>349</v>
+      </c>
+      <c r="C120" s="12" t="s">
+        <v>353</v>
+      </c>
+      <c r="D120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="L120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="M120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="O120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="P120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q120" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="S120" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="T120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="U120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="V120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="W120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="X120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y120" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA120" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="AB118" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC118" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="119" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B119" s="11" t="s">
+      <c r="AB120" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC120" s="11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="121" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A121" s="11"/>
+      <c r="B121" s="11" t="s">
         <v>345</v>
       </c>
-      <c r="C119" s="11" t="s">
-        <v>353</v>
-      </c>
-      <c r="D119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I119" s="6" t="s">
+      <c r="C121" s="12" t="s">
+        <v>357</v>
+      </c>
+      <c r="D121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="E121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="F121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="H121" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="I121" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="J119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="N119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="O119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="R119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="T119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="V119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="W119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="X119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB119" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC119" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="120" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="B120" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="C120" s="11" t="s">
-        <v>354</v>
-      </c>
-      <c r="D120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I120" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="N120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="O120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="R120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="T120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="V120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="W120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="X120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB120" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC120" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="121" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A121" s="11" t="s">
-        <v>356</v>
-      </c>
-      <c r="B121" s="11" t="s">
-        <v>347</v>
-      </c>
-      <c r="C121" s="11" t="s">
-        <v>316</v>
-      </c>
-      <c r="D121" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E121" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F121" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G121" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H121" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I121" s="11" t="s">
-        <v>27</v>
-      </c>
       <c r="J121" s="11" t="s">
         <v>27</v>
       </c>
@@ -18568,7 +18860,7 @@
       <c r="P121" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="Q121" s="11" t="s">
+      <c r="Q121" s="12" t="s">
         <v>27</v>
       </c>
       <c r="R121" s="11" t="s">
@@ -18610,11 +18902,11 @@
     </row>
     <row r="122" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A122" s="11"/>
-      <c r="B122" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="C122" s="11" t="s">
-        <v>348</v>
+      <c r="B122" s="11" t="s">
+        <v>346</v>
+      </c>
+      <c r="C122" s="12" t="s">
+        <v>358</v>
       </c>
       <c r="D122" s="11" t="s">
         <v>27</v>
@@ -18631,7 +18923,7 @@
       <c r="H122" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="I122" s="11" t="s">
+      <c r="I122" s="6" t="s">
         <v>27</v>
       </c>
       <c r="J122" s="11" t="s">
@@ -18696,270 +18988,694 @@
       </c>
     </row>
     <row r="123" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A123" s="11"/>
-      <c r="B123" s="11" t="s">
-        <v>350</v>
-      </c>
-      <c r="C123" s="11" t="s">
-        <v>352</v>
-      </c>
-      <c r="D123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="J123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="N123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="O123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="R123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S123" s="6" t="s">
-        <v>357</v>
-      </c>
-      <c r="T123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="V123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="W123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="X123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y123" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA123" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="AB123" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC123" s="11" t="s">
+      <c r="A123" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="B123" s="12" t="s">
+        <v>347</v>
+      </c>
+      <c r="C123" s="12" t="s">
+        <v>359</v>
+      </c>
+      <c r="D123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="T123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="U123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="W123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="X123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB123" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC123" s="12" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="124" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A124" s="11"/>
-      <c r="B124" s="11" t="s">
-        <v>345</v>
-      </c>
-      <c r="C124" s="11" t="s">
-        <v>353</v>
-      </c>
-      <c r="D124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I124" s="6" t="s">
+      <c r="B124" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="C124" s="12" t="s">
+        <v>360</v>
+      </c>
+      <c r="D124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R124" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="S124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="T124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="U124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="W124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="X124" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y124" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="Z124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA124" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="AB124" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC124" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="125" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A125" s="12" t="s">
+        <v>235</v>
+      </c>
+      <c r="B125" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="C125" s="12" t="s">
+        <v>361</v>
+      </c>
+      <c r="D125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P125" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S125" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="T125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="U125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="W125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="X125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB125" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC125" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="126" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A126" s="12" t="s">
+        <v>236</v>
+      </c>
+      <c r="B126" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="C126" s="12" t="s">
+        <v>362</v>
+      </c>
+      <c r="D126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S126" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="T126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="U126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="W126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="X126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z126" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="AA126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB126" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC126" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="127" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A127" s="12"/>
+      <c r="B127" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="C127" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="D127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I127" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K127" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="J124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="N124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="O124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="R124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="T124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="V124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="W124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="X124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB124" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC124" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="125" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A125" s="11"/>
-      <c r="B125" s="11" t="s">
-        <v>346</v>
-      </c>
-      <c r="C125" s="11" t="s">
-        <v>354</v>
-      </c>
-      <c r="D125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="F125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="G125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="H125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="I125" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="K125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="L125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="M125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="N125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="O125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="P125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="R125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="S125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="T125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="U125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="V125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="W125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="X125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Y125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AB125" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="AC125" s="11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="126" spans="1:29" x14ac:dyDescent="0.25">
-      <c r="A126" s="4" t="s">
-        <v>244</v>
-      </c>
+      <c r="L127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="T127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="U127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="W127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="X127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB127" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC127" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="128" spans="1:29" x14ac:dyDescent="0.25">
+      <c r="A128" s="12"/>
+      <c r="B128" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="C128" s="12" t="s">
+        <v>363</v>
+      </c>
+      <c r="D128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="F128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="G128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="H128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="I128" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="K128" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="L128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="O128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="P128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="R128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="S128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="T128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="U128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="V128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="W128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="X128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB128" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC128" s="12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="129" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C129" s="12"/>
+      <c r="Q129" s="12"/>
+    </row>
+    <row r="130" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C130" s="12"/>
+      <c r="Q130" s="12"/>
+    </row>
+    <row r="131" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C131" s="12"/>
+      <c r="Q131" s="12"/>
+    </row>
+    <row r="132" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C132" s="12"/>
+      <c r="Q132" s="12"/>
+    </row>
+    <row r="133" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q133" s="12"/>
+    </row>
+    <row r="134" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q134" s="12"/>
+    </row>
+    <row r="135" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q135" s="12"/>
+    </row>
+    <row r="136" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q136" s="12"/>
+    </row>
+    <row r="137" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q137" s="12"/>
+    </row>
+    <row r="138" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q138" s="12"/>
+    </row>
+    <row r="139" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q139" s="12"/>
+    </row>
+    <row r="140" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q140" s="12"/>
+    </row>
+    <row r="141" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q141" s="12"/>
+    </row>
+    <row r="142" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q142" s="12"/>
+    </row>
+    <row r="143" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q143" s="12"/>
+    </row>
+    <row r="144" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="Q144" s="12"/>
+    </row>
+    <row r="145" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q145" s="12"/>
+    </row>
+    <row r="146" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q146" s="12"/>
+    </row>
+    <row r="147" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q147" s="12"/>
+    </row>
+    <row r="148" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q148" s="12"/>
+    </row>
+    <row r="149" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q149" s="12"/>
+    </row>
+    <row r="150" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q150" s="12"/>
+    </row>
+    <row r="151" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q151" s="12"/>
+    </row>
+    <row r="152" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q152" s="12"/>
+    </row>
+    <row r="153" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q153" s="12"/>
+    </row>
+    <row r="154" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q154" s="12"/>
+    </row>
+    <row r="155" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q155" s="12"/>
+    </row>
+    <row r="156" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q156" s="12"/>
+    </row>
+    <row r="157" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q157" s="12"/>
+    </row>
+    <row r="158" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q158" s="12"/>
+    </row>
+    <row r="159" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q159" s="12"/>
+    </row>
+    <row r="160" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q160" s="12"/>
+    </row>
+    <row r="161" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q161" s="12"/>
+    </row>
+    <row r="162" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q162" s="12"/>
+    </row>
+    <row r="163" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q163" s="12"/>
+    </row>
+    <row r="164" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q164" s="12"/>
+    </row>
+    <row r="165" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q165" s="12"/>
+    </row>
+    <row r="166" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q166" s="12"/>
+    </row>
+    <row r="167" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q167" s="12"/>
+    </row>
+    <row r="168" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q168" s="12"/>
+    </row>
+    <row r="169" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q169" s="12"/>
+    </row>
+    <row r="170" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q170" s="12"/>
+    </row>
+    <row r="171" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q171" s="12"/>
+    </row>
+    <row r="172" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q172" s="12"/>
+    </row>
+    <row r="173" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q173" s="12"/>
+    </row>
+    <row r="174" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q174" s="12"/>
+    </row>
+    <row r="175" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q175" s="12"/>
+    </row>
+    <row r="176" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q176" s="12"/>
+    </row>
+    <row r="177" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q177" s="12"/>
+    </row>
+    <row r="178" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q178" s="12"/>
+    </row>
+    <row r="179" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q179" s="12"/>
+    </row>
+    <row r="180" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q180" s="12"/>
+    </row>
+    <row r="181" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="Q181" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
New data path implemented
</commit_message>
<xml_diff>
--- a/StateTable/StateTable.xlsx
+++ b/StateTable/StateTable.xlsx
@@ -8563,10 +8563,10 @@
   <dimension ref="A1:AH181"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="D105" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="M105" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B124" sqref="B124"/>
+      <selection pane="bottomRight" activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Do you feel it..
</commit_message>
<xml_diff>
--- a/StateTable/StateTable.xlsx
+++ b/StateTable/StateTable.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5840" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6818" uniqueCount="447">
   <si>
     <t>PC_Enable</t>
   </si>
@@ -1164,9 +1164,6 @@
     <t>1b'0</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>T3</t>
   </si>
   <si>
@@ -1180,6 +1177,195 @@
   </si>
   <si>
     <t>PSR_Clear</t>
+  </si>
+  <si>
+    <t>WRPSR</t>
+  </si>
+  <si>
+    <t>PSR enable</t>
+  </si>
+  <si>
+    <t>PSR Disable</t>
+  </si>
+  <si>
+    <t>WRWIM</t>
+  </si>
+  <si>
+    <t>WIM enable</t>
+  </si>
+  <si>
+    <t>WIM Disable</t>
+  </si>
+  <si>
+    <t>Trapicc</t>
+  </si>
+  <si>
+    <t>Check ET, higher priority, and codition</t>
+  </si>
+  <si>
+    <t>1'b1</t>
+  </si>
+  <si>
+    <t>PS</t>
+  </si>
+  <si>
+    <t>PSR_out[7]</t>
+  </si>
+  <si>
+    <t>PSR Disable, enter superivisor</t>
+  </si>
+  <si>
+    <t>ET</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>PSR disable, disable traps</t>
+  </si>
+  <si>
+    <t>PSR disable, decrement CWP</t>
+  </si>
+  <si>
+    <t>modifying tt</t>
+  </si>
+  <si>
+    <t>4'b0111</t>
+  </si>
+  <si>
+    <t>Save PC and nPC</t>
+  </si>
+  <si>
+    <t>PSR disable, Saving PC</t>
+  </si>
+  <si>
+    <t>4'b0011</t>
+  </si>
+  <si>
+    <t>5'b10001</t>
+  </si>
+  <si>
+    <t>4'b0100</t>
+  </si>
+  <si>
+    <t>5'b10010</t>
+  </si>
+  <si>
+    <t>Jump to trap</t>
+  </si>
+  <si>
+    <t>Disable, PC - &gt; Trap</t>
+  </si>
+  <si>
+    <t>Enable PC</t>
+  </si>
+  <si>
+    <t>Disable PC, nPC + 4</t>
+  </si>
+  <si>
+    <t>4'b0110</t>
+  </si>
+  <si>
+    <t>137</t>
+  </si>
+  <si>
+    <t>138</t>
+  </si>
+  <si>
+    <t>139</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>142</t>
+  </si>
+  <si>
+    <t>143</t>
+  </si>
+  <si>
+    <t>144</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>146</t>
+  </si>
+  <si>
+    <t>147</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>149</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>151</t>
+  </si>
+  <si>
+    <t>152</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
+    <t>154</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>156</t>
+  </si>
+  <si>
+    <t>157</t>
+  </si>
+  <si>
+    <t>158</t>
+  </si>
+  <si>
+    <t>159</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>161</t>
+  </si>
+  <si>
+    <t>162</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>164</t>
+  </si>
+  <si>
+    <t>165</t>
+  </si>
+  <si>
+    <t>166</t>
+  </si>
+  <si>
+    <t>Priority Manager</t>
+  </si>
+  <si>
+    <t>Ifs and elses</t>
+  </si>
+  <si>
+    <t>TBR Disable, Set PS</t>
+  </si>
+  <si>
+    <t>Disable reg, Saving nPC</t>
   </si>
 </sst>
 </file>
@@ -1221,7 +1407,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1248,6 +1434,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1600,41 +1789,41 @@
       <c r="A2" s="3"/>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
       <c r="AB2" s="3"/>
       <c r="AC2" s="3"/>
-      <c r="AD2" s="15" t="s">
+      <c r="AD2" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="15"/>
-      <c r="AH2" s="15"/>
+      <c r="AE2" s="16"/>
+      <c r="AF2" s="16"/>
+      <c r="AG2" s="16"/>
+      <c r="AH2" s="16"/>
     </row>
     <row r="3" spans="1:38" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
@@ -8620,13 +8809,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO178"/>
+  <dimension ref="A1:AR177"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C140" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J27" sqref="J27"/>
+      <selection pane="bottomRight" activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8651,64 +8840,66 @@
     <col min="21" max="21" width="19.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="17.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="16.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="9.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="27" max="30" width="13.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="13.42578125" style="4" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="5.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="9.28515625" style="14" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="10.7109375" style="14" bestFit="1" customWidth="1"/>
     <col min="35" max="36" width="5.7109375" style="14" customWidth="1"/>
-    <col min="37" max="37" width="7" style="14" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="4.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9" style="14" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="42" max="16384" width="9.140625" style="4"/>
+    <col min="37" max="37" width="12.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="38" max="39" width="12.42578125" style="15" customWidth="1"/>
+    <col min="40" max="40" width="7" style="14" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="4.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="12.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="9" style="14" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="10.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="45" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="D1" s="15" t="s">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="D1" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="15"/>
-      <c r="AC1" s="15"/>
-      <c r="AD1" s="15"/>
-      <c r="AE1" s="15"/>
-      <c r="AF1" s="15"/>
-      <c r="AK1" s="15" t="s">
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="16"/>
+      <c r="AC1" s="16"/>
+      <c r="AD1" s="16"/>
+      <c r="AE1" s="16"/>
+      <c r="AF1" s="16"/>
+      <c r="AN1" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="AL1" s="15"/>
-      <c r="AM1" s="15"/>
-      <c r="AN1" s="15"/>
-      <c r="AO1" s="15"/>
-    </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AO1" s="16"/>
+      <c r="AP1" s="16"/>
+      <c r="AQ1" s="16"/>
+      <c r="AR1" s="16"/>
+    </row>
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>198</v>
       </c>
@@ -8755,7 +8946,7 @@
         <v>158</v>
       </c>
       <c r="P2" s="14" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="Q2" s="4" t="s">
         <v>7</v>
@@ -8764,10 +8955,10 @@
         <v>326</v>
       </c>
       <c r="S2" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="T2" s="9" t="s">
         <v>383</v>
-      </c>
-      <c r="T2" s="9" t="s">
-        <v>384</v>
       </c>
       <c r="U2" s="4" t="s">
         <v>153</v>
@@ -8812,28 +9003,37 @@
         <v>17</v>
       </c>
       <c r="AI2" s="14" t="s">
+        <v>379</v>
+      </c>
+      <c r="AJ2" s="14" t="s">
         <v>380</v>
       </c>
-      <c r="AJ2" s="14" t="s">
-        <v>381</v>
-      </c>
-      <c r="AK2" s="14" t="s">
+      <c r="AK2" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="AL2" s="15" t="s">
+        <v>397</v>
+      </c>
+      <c r="AM2" s="15" t="s">
+        <v>396</v>
+      </c>
+      <c r="AN2" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="AL2" s="14" t="s">
+      <c r="AO2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AP2" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="AN2" s="14" t="s">
+      <c r="AQ2" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="AO2" s="14" t="s">
+      <c r="AR2" s="14" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
@@ -8931,7 +9131,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="7" t="s">
         <v>328</v>
       </c>
@@ -9029,13 +9229,16 @@
       <c r="AH4" s="14"/>
       <c r="AI4" s="14"/>
       <c r="AJ4" s="14"/>
-      <c r="AK4" s="14"/>
-      <c r="AL4" s="14"/>
-      <c r="AM4" s="14"/>
+      <c r="AK4" s="15"/>
+      <c r="AL4" s="15"/>
+      <c r="AM4" s="15"/>
       <c r="AN4" s="14"/>
       <c r="AO4" s="14"/>
-    </row>
-    <row r="5" spans="1:41" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AP4" s="14"/>
+      <c r="AQ4" s="14"/>
+      <c r="AR4" s="14"/>
+    </row>
+    <row r="5" spans="1:44" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="9" t="s">
         <v>174</v>
       </c>
@@ -9130,7 +9333,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:41" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:44" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B6" s="9" t="s">
         <v>341</v>
       </c>
@@ -9225,7 +9428,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>28</v>
       </c>
@@ -9323,7 +9526,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7" t="s">
         <v>319</v>
       </c>
@@ -9421,13 +9624,16 @@
       <c r="AH8" s="14"/>
       <c r="AI8" s="14"/>
       <c r="AJ8" s="14"/>
-      <c r="AK8" s="14"/>
-      <c r="AL8" s="14"/>
-      <c r="AM8" s="14"/>
+      <c r="AK8" s="15"/>
+      <c r="AL8" s="15"/>
+      <c r="AM8" s="15"/>
       <c r="AN8" s="14"/>
       <c r="AO8" s="14"/>
-    </row>
-    <row r="9" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AP8" s="14"/>
+      <c r="AQ8" s="14"/>
+      <c r="AR8" s="14"/>
+    </row>
+    <row r="9" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="7" t="s">
         <v>320</v>
       </c>
@@ -9525,13 +9731,16 @@
       <c r="AH9" s="14"/>
       <c r="AI9" s="14"/>
       <c r="AJ9" s="14"/>
-      <c r="AK9" s="14"/>
-      <c r="AL9" s="14"/>
-      <c r="AM9" s="14"/>
+      <c r="AK9" s="15"/>
+      <c r="AL9" s="15"/>
+      <c r="AM9" s="15"/>
       <c r="AN9" s="14"/>
       <c r="AO9" s="14"/>
-    </row>
-    <row r="10" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AP9" s="14"/>
+      <c r="AQ9" s="14"/>
+      <c r="AR9" s="14"/>
+    </row>
+    <row r="10" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="7" t="s">
         <v>323</v>
       </c>
@@ -9629,13 +9838,16 @@
       <c r="AH10" s="14"/>
       <c r="AI10" s="14"/>
       <c r="AJ10" s="14"/>
-      <c r="AK10" s="14"/>
-      <c r="AL10" s="14"/>
-      <c r="AM10" s="14"/>
+      <c r="AK10" s="15"/>
+      <c r="AL10" s="15"/>
+      <c r="AM10" s="15"/>
       <c r="AN10" s="14"/>
       <c r="AO10" s="14"/>
-    </row>
-    <row r="11" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="AP10" s="14"/>
+      <c r="AQ10" s="14"/>
+      <c r="AR10" s="14"/>
+    </row>
+    <row r="11" spans="1:44" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="7" t="s">
         <v>322</v>
       </c>
@@ -9733,13 +9945,16 @@
       <c r="AH11" s="14"/>
       <c r="AI11" s="14"/>
       <c r="AJ11" s="14"/>
-      <c r="AK11" s="14"/>
-      <c r="AL11" s="14"/>
-      <c r="AM11" s="14"/>
+      <c r="AK11" s="15"/>
+      <c r="AL11" s="15"/>
+      <c r="AM11" s="15"/>
       <c r="AN11" s="14"/>
       <c r="AO11" s="14"/>
-    </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="AP11" s="14"/>
+      <c r="AQ11" s="14"/>
+      <c r="AR11" s="14"/>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
@@ -9837,7 +10052,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>163</v>
       </c>
@@ -9932,7 +10147,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>164</v>
       </c>
@@ -10027,7 +10242,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>127</v>
       </c>
@@ -10125,7 +10340,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>171</v>
       </c>
@@ -20220,7 +20435,7 @@
         <v>27</v>
       </c>
       <c r="F122" s="12" t="s">
-        <v>379</v>
+        <v>27</v>
       </c>
       <c r="G122" s="12" t="s">
         <v>27</v>
@@ -20494,300 +20709,3140 @@
       </c>
     </row>
     <row r="125" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="C125" s="13" t="s">
+      <c r="A125" s="15" t="s">
+        <v>384</v>
+      </c>
+      <c r="B125" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="C125" s="15" t="s">
         <v>359</v>
       </c>
+      <c r="D125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U125" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="V125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z125" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="AA125" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB125" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD125" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="AE125" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF125" s="15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="126" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="C126" s="13" t="s">
+      <c r="A126" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B126" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C126" s="15" t="s">
         <v>360</v>
       </c>
-      <c r="R126" s="12"/>
-      <c r="S126" s="14"/>
-      <c r="T126" s="14"/>
+      <c r="D126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q126" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="R126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V126" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="W126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y126" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE126" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF126" s="15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="127" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="C127" s="13" t="s">
+      <c r="A127" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B127" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C127" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="R127" s="12"/>
-      <c r="S127" s="14"/>
-      <c r="T127" s="14"/>
+      <c r="D127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V127" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="W127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC127" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="AD127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE127" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF127" s="15" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="128" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="C128" s="13" t="s">
+      <c r="A128" s="15"/>
+      <c r="B128" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="C128" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="R128" s="12"/>
-      <c r="S128" s="14"/>
-      <c r="T128" s="14"/>
-    </row>
-    <row r="129" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C129" s="13" t="s">
+      <c r="D128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I128" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L128" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="M128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE128" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF128" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="129" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A129" s="15"/>
+      <c r="B129" s="15" t="s">
+        <v>386</v>
+      </c>
+      <c r="C129" s="15" t="s">
         <v>367</v>
       </c>
-      <c r="R129" s="12"/>
-      <c r="S129" s="14"/>
-      <c r="T129" s="14"/>
-    </row>
-    <row r="130" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C130" s="13" t="s">
+      <c r="D129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I129" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L129" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="M129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE129" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF129" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="130" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A130" s="15" t="s">
+        <v>387</v>
+      </c>
+      <c r="B130" s="15" t="s">
+        <v>377</v>
+      </c>
+      <c r="C130" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="R130" s="12"/>
-      <c r="S130" s="14"/>
-      <c r="T130" s="14"/>
-    </row>
-    <row r="131" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C131" s="13" t="s">
+      <c r="D130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U130" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="V130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA130" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB130" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD130" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="AE130" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF130" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="131" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A131" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="B131" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C131" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="R131" s="12"/>
-      <c r="S131" s="14"/>
-      <c r="T131" s="14"/>
-    </row>
-    <row r="132" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C132" s="13" t="s">
+      <c r="D131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q131" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="R131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V131" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="W131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE131" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF131" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="132" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A132" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="B132" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C132" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="R132" s="12"/>
-      <c r="S132" s="14"/>
-      <c r="T132" s="14"/>
-    </row>
-    <row r="133" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C133" s="13" t="s">
+      <c r="D132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V132" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="W132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC132" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="AD132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE132" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF132" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="133" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A133" s="15"/>
+      <c r="B133" s="15" t="s">
+        <v>388</v>
+      </c>
+      <c r="C133" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="R133" s="12"/>
-      <c r="S133" s="14"/>
-      <c r="T133" s="14"/>
-    </row>
-    <row r="134" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C134" s="13" t="s">
+      <c r="D133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I133" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O133" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE133" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF133" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="134" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A134" s="15"/>
+      <c r="B134" s="15" t="s">
+        <v>389</v>
+      </c>
+      <c r="C134" s="15" t="s">
         <v>372</v>
       </c>
-      <c r="R134" s="12"/>
-      <c r="S134" s="14"/>
-      <c r="T134" s="14"/>
-    </row>
-    <row r="135" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C135" s="13" t="s">
+      <c r="D134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I134" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O134" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="P134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE134" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF134" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="135" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A135" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="B135" s="4" t="s">
+        <v>391</v>
+      </c>
+      <c r="C135" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="R135" s="12"/>
-      <c r="S135" s="14"/>
-      <c r="T135" s="14"/>
-    </row>
-    <row r="136" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C136" s="13" t="s">
+      <c r="D135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U135" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="V135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y135" s="6" t="s">
+        <v>392</v>
+      </c>
+      <c r="Z135" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB135" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="AC135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD135" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE135" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF135" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="136" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B136" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="C136" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="R136" s="12"/>
-      <c r="S136" s="14"/>
-      <c r="T136" s="14"/>
-    </row>
-    <row r="137" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C137" s="13" t="s">
+      <c r="D136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q136" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="R136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V136" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="W136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE136" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF136" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="137" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B137" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="C137" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="R137" s="12"/>
-      <c r="S137" s="14"/>
-      <c r="T137" s="14"/>
-    </row>
-    <row r="138" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C138" s="13" t="s">
+      <c r="D137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V137" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="W137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC137" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="AD137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE137" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF137" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="138" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A138" s="4" t="s">
+        <v>400</v>
+      </c>
+      <c r="B138" s="15" t="s">
+        <v>362</v>
+      </c>
+      <c r="C138" s="15" t="s">
         <v>376</v>
       </c>
-      <c r="R138" s="12"/>
-      <c r="S138" s="14"/>
-      <c r="T138" s="14"/>
-    </row>
-    <row r="139" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="R139" s="12"/>
-      <c r="S139" s="14"/>
-      <c r="T139" s="14"/>
-    </row>
-    <row r="140" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="R140" s="12"/>
-      <c r="S140" s="14"/>
-      <c r="T140" s="14"/>
-    </row>
-    <row r="141" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="R141" s="12"/>
-      <c r="S141" s="14"/>
-      <c r="T141" s="14"/>
-    </row>
-    <row r="142" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="R142" s="12"/>
-      <c r="S142" s="14"/>
-      <c r="T142" s="14"/>
-    </row>
-    <row r="143" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="R143" s="12"/>
-      <c r="S143" s="14"/>
-      <c r="T143" s="14"/>
-    </row>
-    <row r="144" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="R144" s="12"/>
-      <c r="S144" s="14"/>
-      <c r="T144" s="14"/>
-    </row>
-    <row r="145" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R145" s="12"/>
-      <c r="S145" s="14"/>
-      <c r="T145" s="14"/>
-    </row>
-    <row r="146" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R146" s="12"/>
-      <c r="S146" s="14"/>
-      <c r="T146" s="14"/>
-    </row>
-    <row r="147" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R147" s="12"/>
-      <c r="S147" s="14"/>
-      <c r="T147" s="14"/>
-    </row>
-    <row r="148" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R148" s="12"/>
-      <c r="S148" s="14"/>
-      <c r="T148" s="14"/>
-    </row>
-    <row r="149" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R149" s="12"/>
-      <c r="S149" s="14"/>
-      <c r="T149" s="14"/>
-    </row>
-    <row r="150" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R150" s="12"/>
-      <c r="S150" s="14"/>
-      <c r="T150" s="14"/>
-    </row>
-    <row r="151" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R151" s="12"/>
-      <c r="S151" s="14"/>
-      <c r="T151" s="14"/>
-    </row>
-    <row r="152" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R152" s="12"/>
-      <c r="S152" s="14"/>
-      <c r="T152" s="14"/>
-    </row>
-    <row r="153" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R153" s="12"/>
-      <c r="S153" s="14"/>
-      <c r="T153" s="14"/>
-    </row>
-    <row r="154" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R154" s="12"/>
-      <c r="S154" s="14"/>
-      <c r="T154" s="14"/>
-    </row>
-    <row r="155" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R155" s="12"/>
-      <c r="S155" s="14"/>
-      <c r="T155" s="14"/>
-    </row>
-    <row r="156" spans="18:20" x14ac:dyDescent="0.25">
+      <c r="D138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I138" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K138" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="L138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE138" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF138" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="139" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B139" s="15" t="s">
+        <v>445</v>
+      </c>
+      <c r="C139" s="15" t="s">
+        <v>413</v>
+      </c>
+      <c r="D139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I139" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K139" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z139" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF139" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK139" s="6" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="140" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B140" s="4" t="s">
+        <v>385</v>
+      </c>
+      <c r="C140" s="15" t="s">
+        <v>414</v>
+      </c>
+      <c r="D140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I140" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M140" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE140" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF140" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="141" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B141" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="C141" s="15" t="s">
+        <v>415</v>
+      </c>
+      <c r="D141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I141" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M141" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z141" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="AA141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF141" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL141" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="142" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B142" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="C142" s="15" t="s">
+        <v>416</v>
+      </c>
+      <c r="D142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I142" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M142" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE142" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF142" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="143" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B143" s="4" t="s">
+        <v>398</v>
+      </c>
+      <c r="C143" s="15" t="s">
+        <v>417</v>
+      </c>
+      <c r="D143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I143" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M143" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z143" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="AA143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF143" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AM143" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="144" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="B144" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="C144" s="15" t="s">
+        <v>418</v>
+      </c>
+      <c r="D144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I144" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M144" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE144" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF144" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="145" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B145" s="15" t="s">
+        <v>399</v>
+      </c>
+      <c r="C145" s="15" t="s">
+        <v>419</v>
+      </c>
+      <c r="D145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I145" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M145" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U145" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="V145" s="6" t="s">
+        <v>401</v>
+      </c>
+      <c r="W145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z145" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD145" s="6" t="s">
+        <v>271</v>
+      </c>
+      <c r="AE145" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF145" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="146" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B146" s="15" t="s">
+        <v>385</v>
+      </c>
+      <c r="C146" s="15" t="s">
+        <v>420</v>
+      </c>
+      <c r="D146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I146" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M146" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="N146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE146" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF146" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="147" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A147" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="B147" s="15" t="s">
+        <v>403</v>
+      </c>
+      <c r="C147" s="15" t="s">
+        <v>421</v>
+      </c>
+      <c r="D147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I147" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M147" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="N147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U147" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="V147" s="6" t="s">
+        <v>404</v>
+      </c>
+      <c r="W147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA147" s="6" t="s">
+        <v>405</v>
+      </c>
+      <c r="AB147" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="AC147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD147" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="AE147" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF147" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="148" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B148" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="C148" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="D148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I148" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE148" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF148" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="149" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B149" s="4" t="s">
+        <v>446</v>
+      </c>
+      <c r="C149" s="15" t="s">
+        <v>423</v>
+      </c>
+      <c r="D149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I149" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V149" s="6" t="s">
+        <v>406</v>
+      </c>
+      <c r="W149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA149" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="AB149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE149" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF149" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="150" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B150" s="15" t="s">
+        <v>344</v>
+      </c>
+      <c r="C150" s="15" t="s">
+        <v>424</v>
+      </c>
+      <c r="D150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I150" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE150" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF150" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="151" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A151" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="B151" s="15" t="s">
+        <v>409</v>
+      </c>
+      <c r="C151" s="15" t="s">
+        <v>425</v>
+      </c>
+      <c r="D151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I151" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X151" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="Y151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE151" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF151" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="152" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B152" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="C152" s="15" t="s">
+        <v>426</v>
+      </c>
+      <c r="D152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E152" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE152" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF152" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="153" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B153" s="15" t="s">
+        <v>411</v>
+      </c>
+      <c r="C153" s="15" t="s">
+        <v>427</v>
+      </c>
+      <c r="D153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E153" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="G153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U153" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="V153" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="W153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE153" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF153" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="154" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B154" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C154" s="15" t="s">
+        <v>428</v>
+      </c>
+      <c r="D154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F154" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE154" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF154" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="155" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B155" s="15" t="s">
+        <v>187</v>
+      </c>
+      <c r="C155" s="15" t="s">
+        <v>429</v>
+      </c>
+      <c r="D155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="E155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F155" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="H155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="I155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="J155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="K155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="O155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="P155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="R155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="S155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="T155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="U155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="V155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="W155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="X155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AB155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AD155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AE155" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF155" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="156" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A156" s="4" t="s">
+        <v>443</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>444</v>
+      </c>
+      <c r="C156" s="15" t="s">
+        <v>430</v>
+      </c>
       <c r="R156" s="12"/>
       <c r="S156" s="14"/>
       <c r="T156" s="14"/>
     </row>
-    <row r="157" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R157" s="12"/>
-      <c r="S157" s="14"/>
-      <c r="T157" s="14"/>
-    </row>
-    <row r="158" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="C157" s="15" t="s">
+        <v>431</v>
+      </c>
+      <c r="P157" s="4"/>
+      <c r="R157" s="4"/>
+      <c r="S157" s="4"/>
+      <c r="T157" s="4"/>
+    </row>
+    <row r="158" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="C158" s="15" t="s">
+        <v>432</v>
+      </c>
       <c r="R158" s="12"/>
       <c r="S158" s="14"/>
       <c r="T158" s="14"/>
     </row>
-    <row r="159" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="C159" s="15" t="s">
+        <v>433</v>
+      </c>
       <c r="R159" s="12"/>
       <c r="S159" s="14"/>
       <c r="T159" s="14"/>
     </row>
-    <row r="160" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="C160" s="15" t="s">
+        <v>434</v>
+      </c>
       <c r="R160" s="12"/>
       <c r="S160" s="14"/>
       <c r="T160" s="14"/>
     </row>
-    <row r="161" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="161" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C161" s="15" t="s">
+        <v>435</v>
+      </c>
       <c r="R161" s="12"/>
       <c r="S161" s="14"/>
       <c r="T161" s="14"/>
     </row>
-    <row r="162" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="162" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C162" s="15" t="s">
+        <v>436</v>
+      </c>
       <c r="R162" s="12"/>
       <c r="S162" s="14"/>
       <c r="T162" s="14"/>
     </row>
-    <row r="163" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="163" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C163" s="15" t="s">
+        <v>437</v>
+      </c>
       <c r="R163" s="12"/>
       <c r="S163" s="14"/>
       <c r="T163" s="14"/>
     </row>
-    <row r="164" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="164" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C164" s="15" t="s">
+        <v>438</v>
+      </c>
       <c r="R164" s="12"/>
       <c r="S164" s="14"/>
       <c r="T164" s="14"/>
     </row>
-    <row r="165" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="165" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C165" s="15" t="s">
+        <v>439</v>
+      </c>
       <c r="R165" s="12"/>
       <c r="S165" s="14"/>
       <c r="T165" s="14"/>
     </row>
-    <row r="166" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="166" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C166" s="15" t="s">
+        <v>440</v>
+      </c>
       <c r="R166" s="12"/>
       <c r="S166" s="14"/>
       <c r="T166" s="14"/>
     </row>
-    <row r="167" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="167" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C167" s="15" t="s">
+        <v>441</v>
+      </c>
       <c r="R167" s="12"/>
       <c r="S167" s="14"/>
       <c r="T167" s="14"/>
     </row>
-    <row r="168" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="168" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C168" s="15" t="s">
+        <v>442</v>
+      </c>
       <c r="R168" s="12"/>
       <c r="S168" s="14"/>
       <c r="T168" s="14"/>
     </row>
-    <row r="169" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="169" spans="3:20" x14ac:dyDescent="0.25">
       <c r="R169" s="12"/>
       <c r="S169" s="14"/>
       <c r="T169" s="14"/>
     </row>
-    <row r="170" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="170" spans="3:20" x14ac:dyDescent="0.25">
       <c r="R170" s="12"/>
       <c r="S170" s="14"/>
       <c r="T170" s="14"/>
     </row>
-    <row r="171" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="171" spans="3:20" x14ac:dyDescent="0.25">
       <c r="R171" s="12"/>
       <c r="S171" s="14"/>
       <c r="T171" s="14"/>
     </row>
-    <row r="172" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="172" spans="3:20" x14ac:dyDescent="0.25">
       <c r="R172" s="12"/>
       <c r="S172" s="14"/>
       <c r="T172" s="14"/>
     </row>
-    <row r="173" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="173" spans="3:20" x14ac:dyDescent="0.25">
       <c r="R173" s="12"/>
       <c r="S173" s="14"/>
       <c r="T173" s="14"/>
     </row>
-    <row r="174" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="174" spans="3:20" x14ac:dyDescent="0.25">
       <c r="R174" s="12"/>
       <c r="S174" s="14"/>
       <c r="T174" s="14"/>
     </row>
-    <row r="175" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="175" spans="3:20" x14ac:dyDescent="0.25">
       <c r="R175" s="12"/>
       <c r="S175" s="14"/>
       <c r="T175" s="14"/>
     </row>
-    <row r="176" spans="18:20" x14ac:dyDescent="0.25">
+    <row r="176" spans="3:20" x14ac:dyDescent="0.25">
       <c r="R176" s="12"/>
       <c r="S176" s="14"/>
       <c r="T176" s="14"/>
@@ -20797,15 +23852,10 @@
       <c r="S177" s="14"/>
       <c r="T177" s="14"/>
     </row>
-    <row r="178" spans="18:20" x14ac:dyDescent="0.25">
-      <c r="R178" s="12"/>
-      <c r="S178" s="14"/>
-      <c r="T178" s="14"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="D1:AF1"/>
-    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AN1:AR1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>